<commit_message>
Fixes an issue with CCS for the cement industry
The formula for calculating the amount of CO2 captured and stored for the cement industry was wrong, leading to negative results.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-direct-air-capture.xlsx
+++ b/premise/data/additional_inventories/lci-direct-air-capture.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="122">
   <si>
     <t>Activity</t>
   </si>
@@ -369,9 +369,6 @@
     <t>copper, anode</t>
   </si>
   <si>
-    <t>Life Cycle Assessment of Direct Air Carbon Capture and Storage with low carbon energy sources, Terlouw et al. 2021 (in review)</t>
-  </si>
-  <si>
     <t>assumptions: uses waste heat and electricity from grid, DAC unit located 1 km away from the synfuel plant, CO2 pressurized to 25 bar</t>
   </si>
   <si>
@@ -379,6 +376,15 @@
   </si>
   <si>
     <t>assumptions: originally in RER. uses waste heat and electricity from grid, DAC unit located 1 km away from the synfuel plant, CO2 pressurized to 25 bar</t>
+  </si>
+  <si>
+    <t>Life cycle assessment of carbon dioxide removal technologies: a critical review. Tom Terlouw, Christian Bauer, Lorenzo Rosa and Marco Mazzotti. 2021. https://doi.org/10.1039/D0EE03757E</t>
+  </si>
+  <si>
+    <t>Represents old infrastructures from ClimeWorks, might be outdated.</t>
+  </si>
+  <si>
+    <t>Timofte A. A Life Cycle Assessment of the Climeworks technology for direct air capture of carbon dioxide, a semester project in the ecological systems design group. Institute of Environmental Engineering of ETH Zurich; 2013.</t>
   </si>
 </sst>
 </file>
@@ -762,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S559"/>
+  <dimension ref="A1:S575"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="H242" sqref="H242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +832,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -834,7 +840,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1174,7 +1180,7 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1182,7 +1188,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1522,7 +1528,7 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -1530,7 +1536,7 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1710,7 +1716,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" s="6">
         <v>0.57799999999999996</v>
@@ -1870,7 +1876,7 @@
         <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -1878,7 +1884,7 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2058,7 +2064,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B77" s="6">
         <v>0.57799999999999996</v>
@@ -2218,7 +2224,7 @@
         <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -2226,7 +2232,7 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2406,7 +2412,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B97" s="6">
         <v>0.57799999999999996</v>
@@ -2566,7 +2572,7 @@
         <v>9</v>
       </c>
       <c r="B107" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
@@ -2574,7 +2580,7 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2754,7 +2760,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B117" s="6">
         <v>0.57799999999999996</v>
@@ -2914,7 +2920,7 @@
         <v>9</v>
       </c>
       <c r="B127" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
@@ -2922,7 +2928,7 @@
         <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3102,7 +3108,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B137" s="6">
         <v>0.57799999999999996</v>
@@ -3262,7 +3268,7 @@
         <v>9</v>
       </c>
       <c r="B147" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
@@ -3270,7 +3276,7 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3450,7 +3456,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B157" s="6">
         <v>0.57799999999999996</v>
@@ -3610,7 +3616,7 @@
         <v>9</v>
       </c>
       <c r="B167" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
@@ -3618,7 +3624,7 @@
         <v>32</v>
       </c>
       <c r="B168" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3798,7 +3804,7 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B177" s="6">
         <v>0.57799999999999996</v>
@@ -3958,7 +3964,7 @@
         <v>9</v>
       </c>
       <c r="B187" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
@@ -3966,7 +3972,7 @@
         <v>32</v>
       </c>
       <c r="B188" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -4146,7 +4152,7 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B197" s="6">
         <v>0.57799999999999996</v>
@@ -4306,7 +4312,7 @@
         <v>9</v>
       </c>
       <c r="B207" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.3">
@@ -4314,7 +4320,7 @@
         <v>32</v>
       </c>
       <c r="B208" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -4494,7 +4500,7 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B217" s="6">
         <v>0.57799999999999996</v>
@@ -4654,7 +4660,7 @@
         <v>9</v>
       </c>
       <c r="B227" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
@@ -4662,7 +4668,7 @@
         <v>32</v>
       </c>
       <c r="B228" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -4842,7 +4848,7 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B237" s="6">
         <v>0.57799999999999996</v>
@@ -5013,110 +5019,68 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A249" s="1" t="s">
-        <v>10</v>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>9</v>
+      </c>
+      <c r="B249" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
+        <v>32</v>
+      </c>
+      <c r="B250" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A251" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
         <v>11</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B252" t="s">
         <v>12</v>
       </c>
-      <c r="C250" t="s">
-        <v>5</v>
-      </c>
-      <c r="D250" t="s">
+      <c r="C252" t="s">
+        <v>5</v>
+      </c>
+      <c r="D252" t="s">
         <v>7</v>
       </c>
-      <c r="E250" t="s">
+      <c r="E252" t="s">
         <v>13</v>
       </c>
-      <c r="F250" t="s">
+      <c r="F252" t="s">
         <v>3</v>
       </c>
-      <c r="G250" t="s">
+      <c r="G252" t="s">
         <v>14</v>
       </c>
-      <c r="H250" t="s">
+      <c r="H252" t="s">
         <v>15</v>
       </c>
-      <c r="I250" t="s">
+      <c r="I252" t="s">
         <v>16</v>
       </c>
-      <c r="J250" t="s">
-        <v>2</v>
-      </c>
-      <c r="K250" t="s">
+      <c r="J252" t="s">
+        <v>2</v>
+      </c>
+      <c r="K252" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="251" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A251" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B251">
-        <v>1</v>
-      </c>
-      <c r="C251" t="s">
-        <v>5</v>
-      </c>
-      <c r="D251" t="s">
-        <v>8</v>
-      </c>
-      <c r="E251" t="s">
-        <v>69</v>
-      </c>
-      <c r="F251" t="s">
-        <v>18</v>
-      </c>
-      <c r="J251" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K251" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="252" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A252" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B252">
-        <v>1.09529E-7</v>
-      </c>
-      <c r="C252" t="s">
-        <v>5</v>
-      </c>
-      <c r="D252" t="s">
-        <v>8</v>
-      </c>
-      <c r="E252" t="s">
-        <v>19</v>
-      </c>
-      <c r="F252" t="s">
-        <v>20</v>
-      </c>
-      <c r="G252">
-        <v>2</v>
-      </c>
-      <c r="H252">
-        <v>-16.027076482571179</v>
-      </c>
-      <c r="I252">
-        <v>0.54930614433405478</v>
-      </c>
-      <c r="K252" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="253" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B253">
-        <v>1.09529E-7</v>
+        <v>1</v>
       </c>
       <c r="C253" t="s">
         <v>5</v>
@@ -5125,19 +5089,13 @@
         <v>8</v>
       </c>
       <c r="E253" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="F253" t="s">
-        <v>20</v>
-      </c>
-      <c r="G253">
-        <v>2</v>
-      </c>
-      <c r="H253">
-        <v>-16.027076482571179</v>
-      </c>
-      <c r="I253">
-        <v>0.54930614433405478</v>
+        <v>18</v>
+      </c>
+      <c r="J253" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K253" t="s">
         <v>70</v>
@@ -5145,7 +5103,7 @@
     </row>
     <row r="254" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B254">
         <v>1.09529E-7</v>
@@ -5177,7 +5135,7 @@
     </row>
     <row r="255" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B255">
         <v>1.09529E-7</v>
@@ -5207,9 +5165,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A256" t="s">
-        <v>75</v>
+    <row r="256" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A256" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B256">
         <v>1.09529E-7</v>
@@ -5239,9 +5197,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A257" t="s">
-        <v>76</v>
+    <row r="257" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A257" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B257">
         <v>1.09529E-7</v>
@@ -5271,9 +5229,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="258" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A258" s="2" t="s">
-        <v>77</v>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>75</v>
       </c>
       <c r="B258">
         <v>1.09529E-7</v>
@@ -5303,272 +5261,212 @@
         <v>70</v>
       </c>
     </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>76</v>
+      </c>
+      <c r="B259">
+        <v>1.09529E-7</v>
+      </c>
+      <c r="C259" t="s">
+        <v>5</v>
+      </c>
+      <c r="D259" t="s">
+        <v>8</v>
+      </c>
+      <c r="E259" t="s">
+        <v>19</v>
+      </c>
+      <c r="F259" t="s">
+        <v>20</v>
+      </c>
+      <c r="G259">
+        <v>2</v>
+      </c>
+      <c r="H259">
+        <v>-16.027076482571179</v>
+      </c>
+      <c r="I259">
+        <v>0.54930614433405478</v>
+      </c>
+      <c r="K259" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="260" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A260" s="1" t="s">
+      <c r="A260" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B260">
+        <v>1.09529E-7</v>
+      </c>
+      <c r="C260" t="s">
+        <v>5</v>
+      </c>
+      <c r="D260" t="s">
+        <v>8</v>
+      </c>
+      <c r="E260" t="s">
+        <v>19</v>
+      </c>
+      <c r="F260" t="s">
+        <v>20</v>
+      </c>
+      <c r="G260">
+        <v>2</v>
+      </c>
+      <c r="H260">
+        <v>-16.027076482571179</v>
+      </c>
+      <c r="I260">
+        <v>0.54930614433405478</v>
+      </c>
+      <c r="K260" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A262" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B260" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A261" t="s">
-        <v>1</v>
-      </c>
-      <c r="B261">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="262" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A262" t="s">
-        <v>2</v>
-      </c>
-      <c r="B262" s="2" t="s">
+      <c r="B262" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>3</v>
-      </c>
-      <c r="B263" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>5</v>
-      </c>
-      <c r="B264" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B265" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="266" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A266" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>5</v>
+      </c>
+      <c r="B266" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B267" t="s">
-        <v>12</v>
-      </c>
-      <c r="C267" t="s">
-        <v>7</v>
-      </c>
-      <c r="D267" t="s">
-        <v>5</v>
-      </c>
-      <c r="E267" t="s">
-        <v>13</v>
-      </c>
-      <c r="F267" t="s">
-        <v>3</v>
-      </c>
-      <c r="G267" t="s">
-        <v>14</v>
-      </c>
-      <c r="H267" t="s">
-        <v>15</v>
-      </c>
-      <c r="I267" t="s">
-        <v>16</v>
-      </c>
-      <c r="J267" t="s">
-        <v>2</v>
-      </c>
-      <c r="K267" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="268" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A268" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B268">
-        <v>1</v>
-      </c>
-      <c r="C268" t="s">
         <v>8</v>
       </c>
-      <c r="D268" t="s">
-        <v>5</v>
-      </c>
-      <c r="E268" t="s">
-        <v>69</v>
-      </c>
-      <c r="F268" t="s">
-        <v>18</v>
-      </c>
-      <c r="J268" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K268" t="s">
-        <v>70</v>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>9</v>
+      </c>
+      <c r="B268" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>78</v>
-      </c>
-      <c r="B269">
-        <v>13000</v>
-      </c>
-      <c r="C269" t="s">
-        <v>79</v>
-      </c>
-      <c r="D269" t="s">
-        <v>6</v>
-      </c>
-      <c r="E269" t="s">
-        <v>80</v>
-      </c>
-      <c r="F269" t="s">
-        <v>20</v>
-      </c>
-      <c r="G269">
-        <v>2</v>
-      </c>
-      <c r="H269">
-        <v>9.4727046364436731</v>
-      </c>
-      <c r="I269">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J269" t="s">
-        <v>81</v>
-      </c>
-      <c r="K269" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A270" t="s">
-        <v>83</v>
-      </c>
-      <c r="B270">
-        <v>500</v>
-      </c>
-      <c r="C270" t="s">
-        <v>8</v>
-      </c>
-      <c r="D270" t="s">
-        <v>6</v>
-      </c>
-      <c r="E270" t="s">
-        <v>80</v>
-      </c>
-      <c r="F270" t="s">
-        <v>20</v>
-      </c>
-      <c r="G270">
-        <v>2</v>
-      </c>
-      <c r="H270">
-        <v>6.2146080984221914</v>
-      </c>
-      <c r="I270">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J270" t="s">
-        <v>84</v>
-      </c>
-      <c r="K270" t="s">
-        <v>82</v>
+        <v>32</v>
+      </c>
+      <c r="B269" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A270" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>85</v>
-      </c>
-      <c r="B271">
-        <v>500</v>
+        <v>11</v>
+      </c>
+      <c r="B271" t="s">
+        <v>12</v>
       </c>
       <c r="C271" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="D271" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E271" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="F271" t="s">
-        <v>20</v>
-      </c>
-      <c r="G271">
-        <v>2</v>
-      </c>
-      <c r="H271">
-        <v>6.2146080984221914</v>
-      </c>
-      <c r="I271">
-        <v>2.439508208471609E-2</v>
+        <v>3</v>
+      </c>
+      <c r="G271" t="s">
+        <v>14</v>
+      </c>
+      <c r="H271" t="s">
+        <v>15</v>
+      </c>
+      <c r="I271" t="s">
+        <v>16</v>
       </c>
       <c r="J271" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="K271" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A272" t="s">
-        <v>88</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A272" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B272">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C272" t="s">
         <v>8</v>
       </c>
       <c r="D272" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E272" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="F272" t="s">
-        <v>20</v>
-      </c>
-      <c r="G272">
-        <v>2</v>
-      </c>
-      <c r="H272">
-        <v>4.7874917427820458</v>
-      </c>
-      <c r="I272">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J272" t="s">
-        <v>89</v>
+        <v>18</v>
+      </c>
+      <c r="J272" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="K272" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B273">
-        <v>15000</v>
+        <v>13000</v>
       </c>
       <c r="C273" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="D273" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E273" t="s">
         <v>80</v>
@@ -5580,1077 +5478,1097 @@
         <v>2</v>
       </c>
       <c r="H273">
-        <v>9.6158054800843473</v>
+        <v>9.4727046364436731</v>
       </c>
       <c r="I273">
-        <v>0.2126338677021721</v>
+        <v>2.439508208471609E-2</v>
       </c>
       <c r="J273" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="K273" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="275" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A275" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B275" s="1" t="s">
-        <v>72</v>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>83</v>
+      </c>
+      <c r="B274">
+        <v>500</v>
+      </c>
+      <c r="C274" t="s">
+        <v>8</v>
+      </c>
+      <c r="D274" t="s">
+        <v>6</v>
+      </c>
+      <c r="E274" t="s">
+        <v>80</v>
+      </c>
+      <c r="F274" t="s">
+        <v>20</v>
+      </c>
+      <c r="G274">
+        <v>2</v>
+      </c>
+      <c r="H274">
+        <v>6.2146080984221914</v>
+      </c>
+      <c r="I274">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J274" t="s">
+        <v>84</v>
+      </c>
+      <c r="K274" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>85</v>
+      </c>
+      <c r="B275">
+        <v>500</v>
+      </c>
+      <c r="C275" t="s">
+        <v>86</v>
+      </c>
+      <c r="D275" t="s">
+        <v>6</v>
+      </c>
+      <c r="E275" t="s">
+        <v>80</v>
+      </c>
+      <c r="F275" t="s">
+        <v>20</v>
+      </c>
+      <c r="G275">
+        <v>2</v>
+      </c>
+      <c r="H275">
+        <v>6.2146080984221914</v>
+      </c>
+      <c r="I275">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J275" t="s">
+        <v>87</v>
+      </c>
+      <c r="K275" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="B276">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="277" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="C276" t="s">
+        <v>8</v>
+      </c>
+      <c r="D276" t="s">
+        <v>6</v>
+      </c>
+      <c r="E276" t="s">
+        <v>80</v>
+      </c>
+      <c r="F276" t="s">
+        <v>20</v>
+      </c>
+      <c r="G276">
+        <v>2</v>
+      </c>
+      <c r="H276">
+        <v>4.7874917427820458</v>
+      </c>
+      <c r="I276">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J276" t="s">
+        <v>89</v>
+      </c>
+      <c r="K276" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>2</v>
-      </c>
-      <c r="B277" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B277">
+        <v>15000</v>
+      </c>
+      <c r="C277" t="s">
+        <v>8</v>
+      </c>
+      <c r="D277" t="s">
+        <v>65</v>
+      </c>
+      <c r="E277" t="s">
+        <v>80</v>
+      </c>
+      <c r="F277" t="s">
+        <v>20</v>
+      </c>
+      <c r="G277">
+        <v>2</v>
+      </c>
+      <c r="H277">
+        <v>9.6158054800843473</v>
+      </c>
+      <c r="I277">
+        <v>0.2126338677021721</v>
+      </c>
+      <c r="J277" t="s">
+        <v>90</v>
+      </c>
+      <c r="K277" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B279" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A278" t="s">
-        <v>3</v>
-      </c>
-      <c r="B278" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A279" t="s">
-        <v>5</v>
-      </c>
-      <c r="B279" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>7</v>
-      </c>
-      <c r="B280" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="B280">
+        <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A281" s="1" t="s">
-        <v>10</v>
+      <c r="A281" t="s">
+        <v>2</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B282" t="s">
-        <v>12</v>
-      </c>
-      <c r="C282" t="s">
-        <v>7</v>
-      </c>
-      <c r="D282" t="s">
-        <v>5</v>
-      </c>
-      <c r="E282" t="s">
-        <v>13</v>
-      </c>
-      <c r="F282" t="s">
-        <v>3</v>
-      </c>
-      <c r="G282" t="s">
-        <v>14</v>
-      </c>
-      <c r="H282" t="s">
-        <v>15</v>
-      </c>
-      <c r="I282" t="s">
-        <v>16</v>
-      </c>
-      <c r="J282" t="s">
-        <v>2</v>
-      </c>
-      <c r="K282" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="283" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A283" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B283">
-        <v>1</v>
-      </c>
-      <c r="C283" t="s">
-        <v>8</v>
-      </c>
-      <c r="D283" t="s">
-        <v>5</v>
-      </c>
-      <c r="E283" t="s">
-        <v>69</v>
-      </c>
-      <c r="F283" t="s">
-        <v>18</v>
-      </c>
-      <c r="J283" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K283" t="s">
-        <v>70</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>5</v>
+      </c>
+      <c r="B283" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>91</v>
-      </c>
-      <c r="B284">
-        <v>1</v>
-      </c>
-      <c r="C284" t="s">
-        <v>22</v>
-      </c>
-      <c r="D284" t="s">
-        <v>5</v>
-      </c>
-      <c r="E284" t="s">
-        <v>19</v>
-      </c>
-      <c r="F284" t="s">
-        <v>20</v>
-      </c>
-      <c r="G284">
-        <v>2</v>
-      </c>
-      <c r="H284">
-        <v>0</v>
-      </c>
-      <c r="I284">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J284" t="s">
-        <v>92</v>
-      </c>
-      <c r="K284" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="B284" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>93</v>
-      </c>
-      <c r="B285">
-        <v>50</v>
-      </c>
-      <c r="C285" t="s">
-        <v>8</v>
-      </c>
-      <c r="D285" t="s">
-        <v>6</v>
-      </c>
-      <c r="E285" t="s">
-        <v>19</v>
-      </c>
-      <c r="F285" t="s">
-        <v>20</v>
-      </c>
-      <c r="G285">
-        <v>2</v>
-      </c>
-      <c r="H285">
-        <v>3.912023005428146</v>
-      </c>
-      <c r="I285">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J285" t="s">
-        <v>94</v>
-      </c>
-      <c r="K285" t="s">
-        <v>82</v>
+        <v>9</v>
+      </c>
+      <c r="B285" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>95</v>
-      </c>
-      <c r="B286">
-        <v>2</v>
-      </c>
-      <c r="C286" t="s">
-        <v>22</v>
-      </c>
-      <c r="D286" t="s">
-        <v>5</v>
-      </c>
-      <c r="E286" t="s">
-        <v>19</v>
-      </c>
-      <c r="F286" t="s">
-        <v>20</v>
-      </c>
-      <c r="G286">
-        <v>2</v>
-      </c>
-      <c r="H286">
-        <v>0.69314718055994529</v>
-      </c>
-      <c r="I286">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J286" t="s">
-        <v>96</v>
-      </c>
-      <c r="K286" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A287" t="s">
-        <v>97</v>
-      </c>
-      <c r="B287">
-        <v>80000</v>
-      </c>
-      <c r="C287" t="s">
-        <v>47</v>
-      </c>
-      <c r="D287" t="s">
-        <v>98</v>
-      </c>
-      <c r="E287" t="s">
-        <v>19</v>
-      </c>
-      <c r="F287" t="s">
-        <v>20</v>
-      </c>
-      <c r="G287">
-        <v>2</v>
-      </c>
-      <c r="H287">
-        <v>11.28978191365602</v>
-      </c>
-      <c r="I287">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J287" t="s">
-        <v>97</v>
-      </c>
-      <c r="K287" t="s">
-        <v>82</v>
+        <v>32</v>
+      </c>
+      <c r="B286" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A287" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>99</v>
-      </c>
-      <c r="B288">
+        <v>11</v>
+      </c>
+      <c r="B288" t="s">
+        <v>12</v>
+      </c>
+      <c r="C288" t="s">
+        <v>7</v>
+      </c>
+      <c r="D288" t="s">
+        <v>5</v>
+      </c>
+      <c r="E288" t="s">
+        <v>13</v>
+      </c>
+      <c r="F288" t="s">
+        <v>3</v>
+      </c>
+      <c r="G288" t="s">
+        <v>14</v>
+      </c>
+      <c r="H288" t="s">
+        <v>15</v>
+      </c>
+      <c r="I288" t="s">
+        <v>16</v>
+      </c>
+      <c r="J288" t="s">
+        <v>2</v>
+      </c>
+      <c r="K288" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A289" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B289">
         <v>1</v>
       </c>
-      <c r="C288" t="s">
-        <v>47</v>
-      </c>
-      <c r="D288" t="s">
-        <v>5</v>
-      </c>
-      <c r="E288" t="s">
+      <c r="C289" t="s">
+        <v>8</v>
+      </c>
+      <c r="D289" t="s">
+        <v>5</v>
+      </c>
+      <c r="E289" t="s">
+        <v>69</v>
+      </c>
+      <c r="F289" t="s">
+        <v>18</v>
+      </c>
+      <c r="J289" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K289" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>91</v>
+      </c>
+      <c r="B290">
+        <v>1</v>
+      </c>
+      <c r="C290" t="s">
+        <v>22</v>
+      </c>
+      <c r="D290" t="s">
+        <v>5</v>
+      </c>
+      <c r="E290" t="s">
         <v>19</v>
       </c>
-      <c r="F288" t="s">
-        <v>20</v>
-      </c>
-      <c r="G288">
-        <v>2</v>
-      </c>
-      <c r="H288">
+      <c r="F290" t="s">
+        <v>20</v>
+      </c>
+      <c r="G290">
+        <v>2</v>
+      </c>
+      <c r="H290">
         <v>0</v>
       </c>
-      <c r="I288">
+      <c r="I290">
         <v>2.439508208471609E-2</v>
       </c>
-      <c r="J288" t="s">
-        <v>99</v>
-      </c>
-      <c r="K288" t="s">
+      <c r="J290" t="s">
+        <v>92</v>
+      </c>
+      <c r="K290" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="290" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A290" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B290" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="B291">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="292" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="C291" t="s">
+        <v>8</v>
+      </c>
+      <c r="D291" t="s">
+        <v>6</v>
+      </c>
+      <c r="E291" t="s">
+        <v>19</v>
+      </c>
+      <c r="F291" t="s">
+        <v>20</v>
+      </c>
+      <c r="G291">
+        <v>2</v>
+      </c>
+      <c r="H291">
+        <v>3.912023005428146</v>
+      </c>
+      <c r="I291">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J291" t="s">
+        <v>94</v>
+      </c>
+      <c r="K291" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>2</v>
-      </c>
-      <c r="B292" s="2" t="s">
-        <v>73</v>
+        <v>95</v>
+      </c>
+      <c r="B292">
+        <v>2</v>
+      </c>
+      <c r="C292" t="s">
+        <v>22</v>
+      </c>
+      <c r="D292" t="s">
+        <v>5</v>
+      </c>
+      <c r="E292" t="s">
+        <v>19</v>
+      </c>
+      <c r="F292" t="s">
+        <v>20</v>
+      </c>
+      <c r="G292">
+        <v>2</v>
+      </c>
+      <c r="H292">
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="I292">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J292" t="s">
+        <v>96</v>
+      </c>
+      <c r="K292" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>3</v>
-      </c>
-      <c r="B293" t="s">
-        <v>4</v>
+        <v>97</v>
+      </c>
+      <c r="B293">
+        <v>80000</v>
+      </c>
+      <c r="C293" t="s">
+        <v>47</v>
+      </c>
+      <c r="D293" t="s">
+        <v>98</v>
+      </c>
+      <c r="E293" t="s">
+        <v>19</v>
+      </c>
+      <c r="F293" t="s">
+        <v>20</v>
+      </c>
+      <c r="G293">
+        <v>2</v>
+      </c>
+      <c r="H293">
+        <v>11.28978191365602</v>
+      </c>
+      <c r="I293">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J293" t="s">
+        <v>97</v>
+      </c>
+      <c r="K293" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>5</v>
-      </c>
-      <c r="B294" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A295" t="s">
-        <v>7</v>
-      </c>
-      <c r="B295" t="s">
-        <v>8</v>
+        <v>99</v>
+      </c>
+      <c r="B294">
+        <v>1</v>
+      </c>
+      <c r="C294" t="s">
+        <v>47</v>
+      </c>
+      <c r="D294" t="s">
+        <v>5</v>
+      </c>
+      <c r="E294" t="s">
+        <v>19</v>
+      </c>
+      <c r="F294" t="s">
+        <v>20</v>
+      </c>
+      <c r="G294">
+        <v>2</v>
+      </c>
+      <c r="H294">
+        <v>0</v>
+      </c>
+      <c r="I294">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J294" t="s">
+        <v>99</v>
+      </c>
+      <c r="K294" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="296" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>11</v>
-      </c>
-      <c r="B297" t="s">
-        <v>12</v>
-      </c>
-      <c r="C297" t="s">
-        <v>7</v>
-      </c>
-      <c r="D297" t="s">
-        <v>5</v>
-      </c>
-      <c r="E297" t="s">
-        <v>13</v>
-      </c>
-      <c r="F297" t="s">
-        <v>3</v>
-      </c>
-      <c r="G297" t="s">
-        <v>14</v>
-      </c>
-      <c r="H297" t="s">
-        <v>15</v>
-      </c>
-      <c r="I297" t="s">
-        <v>16</v>
-      </c>
-      <c r="J297" t="s">
-        <v>2</v>
-      </c>
-      <c r="K297" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="B297">
+        <v>1</v>
       </c>
     </row>
     <row r="298" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A298" s="2" t="s">
+      <c r="A298" t="s">
+        <v>2</v>
+      </c>
+      <c r="B298" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B298">
-        <v>1</v>
-      </c>
-      <c r="C298" t="s">
-        <v>8</v>
-      </c>
-      <c r="D298" t="s">
-        <v>5</v>
-      </c>
-      <c r="E298" t="s">
-        <v>69</v>
-      </c>
-      <c r="F298" t="s">
-        <v>18</v>
-      </c>
-      <c r="J298" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K298" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>83</v>
-      </c>
-      <c r="B299">
-        <v>854</v>
-      </c>
-      <c r="C299" t="s">
-        <v>8</v>
-      </c>
-      <c r="D299" t="s">
-        <v>6</v>
-      </c>
-      <c r="E299" t="s">
-        <v>19</v>
-      </c>
-      <c r="F299" t="s">
-        <v>20</v>
-      </c>
-      <c r="G299">
-        <v>2</v>
-      </c>
-      <c r="H299">
-        <v>6.7499311937885702</v>
-      </c>
-      <c r="I299">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J299" t="s">
-        <v>84</v>
-      </c>
-      <c r="K299" t="s">
-        <v>82</v>
+        <v>3</v>
+      </c>
+      <c r="B299" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>85</v>
-      </c>
-      <c r="B300">
-        <v>454</v>
-      </c>
-      <c r="C300" t="s">
-        <v>86</v>
-      </c>
-      <c r="D300" t="s">
-        <v>6</v>
-      </c>
-      <c r="E300" t="s">
-        <v>19</v>
-      </c>
-      <c r="F300" t="s">
-        <v>20</v>
-      </c>
-      <c r="G300">
-        <v>2</v>
-      </c>
-      <c r="H300">
-        <v>6.1180971980413483</v>
-      </c>
-      <c r="I300">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J300" t="s">
-        <v>87</v>
-      </c>
-      <c r="K300" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="302" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A302" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B302" s="1" t="s">
-        <v>74</v>
+        <v>5</v>
+      </c>
+      <c r="B300" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>7</v>
+      </c>
+      <c r="B301" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>9</v>
+      </c>
+      <c r="B302" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>1</v>
-      </c>
-      <c r="B303">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="B303" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="304" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A304" t="s">
-        <v>2</v>
-      </c>
-      <c r="B304" s="2" t="s">
-        <v>74</v>
+      <c r="A304" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
+        <v>11</v>
+      </c>
+      <c r="B305" t="s">
+        <v>12</v>
+      </c>
+      <c r="C305" t="s">
+        <v>7</v>
+      </c>
+      <c r="D305" t="s">
+        <v>5</v>
+      </c>
+      <c r="E305" t="s">
+        <v>13</v>
+      </c>
+      <c r="F305" t="s">
         <v>3</v>
       </c>
-      <c r="B305" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A306" t="s">
-        <v>5</v>
-      </c>
-      <c r="B306" t="s">
-        <v>5</v>
+      <c r="G305" t="s">
+        <v>14</v>
+      </c>
+      <c r="H305" t="s">
+        <v>15</v>
+      </c>
+      <c r="I305" t="s">
+        <v>16</v>
+      </c>
+      <c r="J305" t="s">
+        <v>2</v>
+      </c>
+      <c r="K305" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A306" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B306">
+        <v>1</v>
+      </c>
+      <c r="C306" t="s">
+        <v>8</v>
+      </c>
+      <c r="D306" t="s">
+        <v>5</v>
+      </c>
+      <c r="E306" t="s">
+        <v>69</v>
+      </c>
+      <c r="F306" t="s">
+        <v>18</v>
+      </c>
+      <c r="J306" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K306" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>7</v>
-      </c>
-      <c r="B307" t="s">
+        <v>83</v>
+      </c>
+      <c r="B307">
+        <v>854</v>
+      </c>
+      <c r="C307" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="308" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A308" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A309" t="s">
-        <v>11</v>
-      </c>
-      <c r="B309" t="s">
-        <v>12</v>
-      </c>
-      <c r="C309" t="s">
-        <v>7</v>
-      </c>
-      <c r="D309" t="s">
-        <v>5</v>
-      </c>
-      <c r="E309" t="s">
-        <v>13</v>
-      </c>
-      <c r="F309" t="s">
-        <v>3</v>
-      </c>
-      <c r="G309" t="s">
-        <v>14</v>
-      </c>
-      <c r="H309" t="s">
-        <v>15</v>
-      </c>
-      <c r="I309" t="s">
-        <v>16</v>
-      </c>
-      <c r="J309" t="s">
-        <v>2</v>
-      </c>
-      <c r="K309" t="s">
-        <v>17</v>
+      <c r="D307" t="s">
+        <v>6</v>
+      </c>
+      <c r="E307" t="s">
+        <v>19</v>
+      </c>
+      <c r="F307" t="s">
+        <v>20</v>
+      </c>
+      <c r="G307">
+        <v>2</v>
+      </c>
+      <c r="H307">
+        <v>6.7499311937885702</v>
+      </c>
+      <c r="I307">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J307" t="s">
+        <v>84</v>
+      </c>
+      <c r="K307" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>85</v>
+      </c>
+      <c r="B308">
+        <v>454</v>
+      </c>
+      <c r="C308" t="s">
+        <v>86</v>
+      </c>
+      <c r="D308" t="s">
+        <v>6</v>
+      </c>
+      <c r="E308" t="s">
+        <v>19</v>
+      </c>
+      <c r="F308" t="s">
+        <v>20</v>
+      </c>
+      <c r="G308">
+        <v>2</v>
+      </c>
+      <c r="H308">
+        <v>6.1180971980413483</v>
+      </c>
+      <c r="I308">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J308" t="s">
+        <v>87</v>
+      </c>
+      <c r="K308" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="310" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A310" s="2" t="s">
+      <c r="A310" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B310" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B310">
-        <v>1</v>
-      </c>
-      <c r="C310" t="s">
-        <v>8</v>
-      </c>
-      <c r="D310" t="s">
-        <v>5</v>
-      </c>
-      <c r="E310" t="s">
-        <v>69</v>
-      </c>
-      <c r="F310" t="s">
-        <v>18</v>
-      </c>
-      <c r="K310" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="B311">
-        <v>9000</v>
-      </c>
-      <c r="C311" t="s">
-        <v>8</v>
-      </c>
-      <c r="D311" t="s">
-        <v>6</v>
-      </c>
-      <c r="E311" t="s">
-        <v>19</v>
-      </c>
-      <c r="F311" t="s">
-        <v>20</v>
-      </c>
-      <c r="G311">
-        <v>2</v>
-      </c>
-      <c r="H311">
-        <v>9000</v>
-      </c>
-      <c r="I311">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J311" t="s">
-        <v>101</v>
-      </c>
-      <c r="K311" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>102</v>
-      </c>
-      <c r="B312">
-        <v>3.54</v>
-      </c>
-      <c r="C312" t="s">
-        <v>47</v>
-      </c>
-      <c r="D312" t="s">
-        <v>6</v>
-      </c>
-      <c r="E312" t="s">
-        <v>19</v>
-      </c>
-      <c r="F312" t="s">
-        <v>20</v>
-      </c>
-      <c r="G312">
-        <v>2</v>
-      </c>
-      <c r="H312">
-        <v>1.2641267271456831</v>
-      </c>
-      <c r="I312">
-        <v>5.6664342653501683E-2</v>
-      </c>
-      <c r="J312" t="s">
-        <v>103</v>
-      </c>
-      <c r="K312" t="s">
-        <v>82</v>
+        <v>2</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="313" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>104</v>
-      </c>
-      <c r="B313">
-        <v>1180</v>
-      </c>
-      <c r="C313" t="s">
-        <v>105</v>
-      </c>
-      <c r="D313" t="s">
-        <v>6</v>
-      </c>
-      <c r="E313" t="s">
-        <v>19</v>
-      </c>
-      <c r="F313" t="s">
-        <v>20</v>
-      </c>
-      <c r="G313">
-        <v>2</v>
-      </c>
-      <c r="H313">
-        <v>7.0732697174597101</v>
-      </c>
-      <c r="I313">
-        <v>5.6664342653501683E-2</v>
-      </c>
-      <c r="J313" t="s">
-        <v>106</v>
-      </c>
-      <c r="K313" t="s">
-        <v>82</v>
+        <v>3</v>
+      </c>
+      <c r="B313" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>85</v>
-      </c>
-      <c r="B314">
-        <v>1180</v>
-      </c>
-      <c r="C314" t="s">
-        <v>86</v>
-      </c>
-      <c r="D314" t="s">
-        <v>6</v>
-      </c>
-      <c r="E314" t="s">
-        <v>19</v>
-      </c>
-      <c r="F314" t="s">
-        <v>20</v>
-      </c>
-      <c r="G314">
-        <v>2</v>
-      </c>
-      <c r="H314">
-        <v>7.0732697174597101</v>
-      </c>
-      <c r="I314">
-        <v>5.6664342653501683E-2</v>
-      </c>
-      <c r="J314" t="s">
-        <v>87</v>
-      </c>
-      <c r="K314" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="B314" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>107</v>
-      </c>
-      <c r="B315">
-        <v>1418</v>
-      </c>
-      <c r="C315" t="s">
-        <v>47</v>
-      </c>
-      <c r="D315" t="s">
-        <v>65</v>
-      </c>
-      <c r="E315" t="s">
-        <v>19</v>
-      </c>
-      <c r="F315" t="s">
-        <v>20</v>
-      </c>
-      <c r="G315">
-        <v>2</v>
-      </c>
-      <c r="H315">
-        <v>7.2570027070920728</v>
-      </c>
-      <c r="I315">
-        <v>5.6664342653501683E-2</v>
-      </c>
-      <c r="J315" t="s">
-        <v>108</v>
-      </c>
-      <c r="K315" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="B315" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>90</v>
-      </c>
-      <c r="B316">
-        <v>1000</v>
-      </c>
-      <c r="C316" t="s">
-        <v>8</v>
-      </c>
-      <c r="D316" t="s">
-        <v>65</v>
-      </c>
-      <c r="E316" t="s">
-        <v>19</v>
-      </c>
-      <c r="F316" t="s">
-        <v>20</v>
-      </c>
-      <c r="G316">
-        <v>2</v>
-      </c>
-      <c r="H316">
-        <v>6.9077552789821368</v>
-      </c>
-      <c r="I316">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J316" t="s">
-        <v>90</v>
-      </c>
-      <c r="K316" t="s">
-        <v>82</v>
+        <v>9</v>
+      </c>
+      <c r="B316" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>90</v>
-      </c>
-      <c r="B317">
-        <v>118</v>
-      </c>
-      <c r="C317" t="s">
-        <v>8</v>
-      </c>
-      <c r="D317" t="s">
-        <v>65</v>
-      </c>
-      <c r="E317" t="s">
-        <v>19</v>
-      </c>
-      <c r="F317" t="s">
-        <v>20</v>
-      </c>
-      <c r="G317">
-        <v>2</v>
-      </c>
-      <c r="H317">
-        <v>4.7706846244656651</v>
-      </c>
-      <c r="I317">
-        <v>5.6664342653501683E-2</v>
-      </c>
-      <c r="J317" t="s">
-        <v>90</v>
-      </c>
-      <c r="K317" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="319" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A319" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B319" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A320" t="s">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="B317" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="318" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A318" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
+        <v>11</v>
+      </c>
+      <c r="B319" t="s">
+        <v>12</v>
+      </c>
+      <c r="C319" t="s">
+        <v>7</v>
+      </c>
+      <c r="D319" t="s">
+        <v>5</v>
+      </c>
+      <c r="E319" t="s">
+        <v>13</v>
+      </c>
+      <c r="F319" t="s">
+        <v>3</v>
+      </c>
+      <c r="G319" t="s">
+        <v>14</v>
+      </c>
+      <c r="H319" t="s">
+        <v>15</v>
+      </c>
+      <c r="I319" t="s">
+        <v>16</v>
+      </c>
+      <c r="J319" t="s">
+        <v>2</v>
+      </c>
+      <c r="K319" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="320" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A320" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B320">
         <v>1</v>
       </c>
+      <c r="C320" t="s">
+        <v>8</v>
+      </c>
+      <c r="D320" t="s">
+        <v>5</v>
+      </c>
+      <c r="E320" t="s">
+        <v>69</v>
+      </c>
+      <c r="F320" t="s">
+        <v>18</v>
+      </c>
+      <c r="K320" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="321" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>2</v>
-      </c>
-      <c r="B321" t="s">
-        <v>75</v>
+        <v>100</v>
+      </c>
+      <c r="B321">
+        <v>9000</v>
+      </c>
+      <c r="C321" t="s">
+        <v>8</v>
+      </c>
+      <c r="D321" t="s">
+        <v>6</v>
+      </c>
+      <c r="E321" t="s">
+        <v>19</v>
+      </c>
+      <c r="F321" t="s">
+        <v>20</v>
+      </c>
+      <c r="G321">
+        <v>2</v>
+      </c>
+      <c r="H321">
+        <v>9000</v>
+      </c>
+      <c r="I321">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J321" t="s">
+        <v>101</v>
+      </c>
+      <c r="K321" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="322" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>3</v>
-      </c>
-      <c r="B322" t="s">
-        <v>4</v>
+        <v>102</v>
+      </c>
+      <c r="B322">
+        <v>3.54</v>
+      </c>
+      <c r="C322" t="s">
+        <v>47</v>
+      </c>
+      <c r="D322" t="s">
+        <v>6</v>
+      </c>
+      <c r="E322" t="s">
+        <v>19</v>
+      </c>
+      <c r="F322" t="s">
+        <v>20</v>
+      </c>
+      <c r="G322">
+        <v>2</v>
+      </c>
+      <c r="H322">
+        <v>1.2641267271456831</v>
+      </c>
+      <c r="I322">
+        <v>5.6664342653501683E-2</v>
+      </c>
+      <c r="J322" t="s">
+        <v>103</v>
+      </c>
+      <c r="K322" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="323" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>5</v>
-      </c>
-      <c r="B323" t="s">
-        <v>5</v>
+        <v>104</v>
+      </c>
+      <c r="B323">
+        <v>1180</v>
+      </c>
+      <c r="C323" t="s">
+        <v>105</v>
+      </c>
+      <c r="D323" t="s">
+        <v>6</v>
+      </c>
+      <c r="E323" t="s">
+        <v>19</v>
+      </c>
+      <c r="F323" t="s">
+        <v>20</v>
+      </c>
+      <c r="G323">
+        <v>2</v>
+      </c>
+      <c r="H323">
+        <v>7.0732697174597101</v>
+      </c>
+      <c r="I323">
+        <v>5.6664342653501683E-2</v>
+      </c>
+      <c r="J323" t="s">
+        <v>106</v>
+      </c>
+      <c r="K323" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="324" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>7</v>
-      </c>
-      <c r="B324" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="325" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A325" s="1" t="s">
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="B324">
+        <v>1180</v>
+      </c>
+      <c r="C324" t="s">
+        <v>86</v>
+      </c>
+      <c r="D324" t="s">
+        <v>6</v>
+      </c>
+      <c r="E324" t="s">
+        <v>19</v>
+      </c>
+      <c r="F324" t="s">
+        <v>20</v>
+      </c>
+      <c r="G324">
+        <v>2</v>
+      </c>
+      <c r="H324">
+        <v>7.0732697174597101</v>
+      </c>
+      <c r="I324">
+        <v>5.6664342653501683E-2</v>
+      </c>
+      <c r="J324" t="s">
+        <v>87</v>
+      </c>
+      <c r="K324" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>107</v>
+      </c>
+      <c r="B325">
+        <v>1418</v>
+      </c>
+      <c r="C325" t="s">
+        <v>47</v>
+      </c>
+      <c r="D325" t="s">
+        <v>65</v>
+      </c>
+      <c r="E325" t="s">
+        <v>19</v>
+      </c>
+      <c r="F325" t="s">
+        <v>20</v>
+      </c>
+      <c r="G325">
+        <v>2</v>
+      </c>
+      <c r="H325">
+        <v>7.2570027070920728</v>
+      </c>
+      <c r="I325">
+        <v>5.6664342653501683E-2</v>
+      </c>
+      <c r="J325" t="s">
+        <v>108</v>
+      </c>
+      <c r="K325" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="326" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>11</v>
-      </c>
-      <c r="B326" t="s">
-        <v>12</v>
+        <v>90</v>
+      </c>
+      <c r="B326">
+        <v>1000</v>
       </c>
       <c r="C326" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D326" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="E326" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F326" t="s">
-        <v>3</v>
-      </c>
-      <c r="G326" t="s">
-        <v>14</v>
-      </c>
-      <c r="H326" t="s">
-        <v>15</v>
-      </c>
-      <c r="I326" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="G326">
+        <v>2</v>
+      </c>
+      <c r="H326">
+        <v>6.9077552789821368</v>
+      </c>
+      <c r="I326">
+        <v>2.439508208471609E-2</v>
       </c>
       <c r="J326" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="K326" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
     </row>
     <row r="327" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B327">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="C327" t="s">
         <v>8</v>
       </c>
       <c r="D327" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="E327" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="F327" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="G327">
+        <v>2</v>
+      </c>
+      <c r="H327">
+        <v>4.7706846244656651</v>
+      </c>
+      <c r="I327">
+        <v>5.6664342653501683E-2</v>
       </c>
       <c r="J327" t="s">
+        <v>90</v>
+      </c>
+      <c r="K327" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A329" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B329" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K327" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A328" t="s">
-        <v>85</v>
-      </c>
-      <c r="B328">
-        <v>2000</v>
-      </c>
-      <c r="C328" t="s">
-        <v>86</v>
-      </c>
-      <c r="D328" t="s">
-        <v>6</v>
-      </c>
-      <c r="E328" t="s">
-        <v>19</v>
-      </c>
-      <c r="F328" t="s">
-        <v>20</v>
-      </c>
-      <c r="G328">
-        <v>2</v>
-      </c>
-      <c r="H328">
-        <v>2000</v>
-      </c>
-      <c r="I328">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J328" t="s">
-        <v>87</v>
-      </c>
-      <c r="K328" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A329" t="s">
-        <v>90</v>
-      </c>
-      <c r="B329">
-        <v>2000</v>
-      </c>
-      <c r="C329" t="s">
-        <v>8</v>
-      </c>
-      <c r="D329" t="s">
-        <v>65</v>
-      </c>
-      <c r="E329" t="s">
-        <v>19</v>
-      </c>
-      <c r="F329" t="s">
-        <v>20</v>
-      </c>
-      <c r="G329">
-        <v>2</v>
-      </c>
-      <c r="H329">
-        <v>7.6009024595420822</v>
-      </c>
-      <c r="I329">
-        <v>0.3465735902799727</v>
-      </c>
-      <c r="J329" t="s">
-        <v>90</v>
-      </c>
-      <c r="K329" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="331" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A331" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B331" s="1" t="s">
-        <v>76</v>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>1</v>
+      </c>
+      <c r="B330">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>2</v>
+      </c>
+      <c r="B331" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="332" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>1</v>
-      </c>
-      <c r="B332">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B332" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="333" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B333" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
     </row>
     <row r="334" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B334" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="335" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B335" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="336" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B336" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
     </row>
     <row r="337" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -6695,7 +6613,7 @@
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B339">
         <v>1</v>
@@ -6713,7 +6631,7 @@
         <v>18</v>
       </c>
       <c r="J339" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K339" t="s">
         <v>70</v>
@@ -6721,16 +6639,16 @@
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="B340">
-        <v>0.17</v>
+        <v>2000</v>
       </c>
       <c r="C340" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="D340" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E340" t="s">
         <v>19</v>
@@ -6742,13 +6660,13 @@
         <v>2</v>
       </c>
       <c r="H340">
-        <v>-1.771956841931875</v>
+        <v>2000</v>
       </c>
       <c r="I340">
-        <v>0.54930614433405478</v>
+        <v>2.439508208471609E-2</v>
       </c>
       <c r="J340" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="K340" t="s">
         <v>82</v>
@@ -6756,16 +6674,16 @@
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B341">
-        <v>125</v>
+        <v>2000</v>
       </c>
       <c r="C341" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D341" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="E341" t="s">
         <v>19</v>
@@ -6777,214 +6695,160 @@
         <v>2</v>
       </c>
       <c r="H341">
-        <v>4.8283137373023024</v>
+        <v>7.6009024595420822</v>
       </c>
       <c r="I341">
-        <v>0.54930614433405478</v>
+        <v>0.3465735902799727</v>
       </c>
       <c r="J341" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="K341" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A342" t="s">
-        <v>113</v>
-      </c>
-      <c r="B342">
-        <v>818</v>
-      </c>
-      <c r="C342" t="s">
-        <v>8</v>
-      </c>
-      <c r="D342" t="s">
-        <v>6</v>
-      </c>
-      <c r="E342" t="s">
-        <v>19</v>
-      </c>
-      <c r="F342" t="s">
-        <v>20</v>
-      </c>
-      <c r="G342">
-        <v>2</v>
-      </c>
-      <c r="H342">
-        <v>6.7068623366027467</v>
-      </c>
-      <c r="I342">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J342" t="s">
-        <v>87</v>
-      </c>
-      <c r="K342" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="344" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A344" s="1" t="s">
+    <row r="343" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A343" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B344" s="1" t="s">
-        <v>77</v>
+      <c r="B343" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>1</v>
+      </c>
+      <c r="B344">
+        <v>1</v>
       </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>1</v>
-      </c>
-      <c r="B345">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="346" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="B345" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>2</v>
-      </c>
-      <c r="B346" s="2" t="s">
-        <v>77</v>
+        <v>3</v>
+      </c>
+      <c r="B346" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B347" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B348" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
+        <v>9</v>
+      </c>
+      <c r="B349" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>32</v>
+      </c>
+      <c r="B350" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A351" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>11</v>
+      </c>
+      <c r="B352" t="s">
+        <v>12</v>
+      </c>
+      <c r="C352" t="s">
         <v>7</v>
       </c>
-      <c r="B349" t="s">
+      <c r="D352" t="s">
+        <v>5</v>
+      </c>
+      <c r="E352" t="s">
+        <v>13</v>
+      </c>
+      <c r="F352" t="s">
+        <v>3</v>
+      </c>
+      <c r="G352" t="s">
+        <v>14</v>
+      </c>
+      <c r="H352" t="s">
+        <v>15</v>
+      </c>
+      <c r="I352" t="s">
+        <v>16</v>
+      </c>
+      <c r="J352" t="s">
+        <v>2</v>
+      </c>
+      <c r="K352" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>76</v>
+      </c>
+      <c r="B353">
+        <v>1</v>
+      </c>
+      <c r="C353" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="350" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A350" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A351" t="s">
-        <v>11</v>
-      </c>
-      <c r="B351" t="s">
-        <v>12</v>
-      </c>
-      <c r="C351" t="s">
-        <v>7</v>
-      </c>
-      <c r="D351" t="s">
-        <v>5</v>
-      </c>
-      <c r="E351" t="s">
-        <v>13</v>
-      </c>
-      <c r="F351" t="s">
-        <v>3</v>
-      </c>
-      <c r="G351" t="s">
-        <v>14</v>
-      </c>
-      <c r="H351" t="s">
-        <v>15</v>
-      </c>
-      <c r="I351" t="s">
-        <v>16</v>
-      </c>
-      <c r="J351" t="s">
-        <v>2</v>
-      </c>
-      <c r="K351" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="352" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A352" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B352">
-        <v>1</v>
-      </c>
-      <c r="C352" t="s">
+      <c r="D353" t="s">
+        <v>5</v>
+      </c>
+      <c r="E353" t="s">
+        <v>69</v>
+      </c>
+      <c r="F353" t="s">
+        <v>18</v>
+      </c>
+      <c r="J353" t="s">
+        <v>76</v>
+      </c>
+      <c r="K353" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>109</v>
+      </c>
+      <c r="B354">
+        <v>0.17</v>
+      </c>
+      <c r="C354" t="s">
         <v>8</v>
       </c>
-      <c r="D352" t="s">
-        <v>5</v>
-      </c>
-      <c r="E352" t="s">
-        <v>69</v>
-      </c>
-      <c r="F352" t="s">
-        <v>18</v>
-      </c>
-      <c r="J352" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K352" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="353" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A353" t="s">
-        <v>114</v>
-      </c>
-      <c r="B353">
-        <v>97.5</v>
-      </c>
-      <c r="C353" t="s">
-        <v>61</v>
-      </c>
-      <c r="D353" t="s">
-        <v>6</v>
-      </c>
-      <c r="E353" t="s">
-        <v>19</v>
-      </c>
-      <c r="F353" t="s">
-        <v>20</v>
-      </c>
-      <c r="G353">
-        <v>2</v>
-      </c>
-      <c r="H353">
-        <v>4.5798523780038014</v>
-      </c>
-      <c r="I353">
-        <v>2.439508208471609E-2</v>
-      </c>
-      <c r="J353" t="s">
-        <v>115</v>
-      </c>
-      <c r="K353" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="354" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A354" t="s">
-        <v>85</v>
-      </c>
-      <c r="B354">
-        <v>3000</v>
-      </c>
-      <c r="C354" t="s">
-        <v>86</v>
-      </c>
       <c r="D354" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E354" t="s">
         <v>19</v>
@@ -6996,30 +6860,30 @@
         <v>2</v>
       </c>
       <c r="H354">
-        <v>8.0063675676502459</v>
+        <v>-1.771956841931875</v>
       </c>
       <c r="I354">
-        <v>2.439508208471609E-2</v>
+        <v>0.54930614433405478</v>
       </c>
       <c r="J354" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="K354" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="355" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="B355">
-        <v>52.5</v>
+        <v>125</v>
       </c>
       <c r="C355" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="D355" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E355" t="s">
         <v>19</v>
@@ -7031,30 +6895,30 @@
         <v>2</v>
       </c>
       <c r="H355">
-        <v>3.9608131695975781</v>
+        <v>4.8283137373023024</v>
       </c>
       <c r="I355">
-        <v>2.439508208471609E-2</v>
+        <v>0.54930614433405478</v>
       </c>
       <c r="J355" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="K355" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="356" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B356">
-        <v>4000</v>
+        <v>818</v>
       </c>
       <c r="C356" t="s">
         <v>8</v>
       </c>
       <c r="D356" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E356" t="s">
         <v>19</v>
@@ -7066,51 +6930,287 @@
         <v>2</v>
       </c>
       <c r="H356">
-        <v>8.2940496401020276</v>
+        <v>6.7068623366027467</v>
       </c>
       <c r="I356">
-        <v>0.3465735902799727</v>
+        <v>2.439508208471609E-2</v>
       </c>
       <c r="J356" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K356" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="362" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A362" s="1"/>
-    </row>
-    <row r="364" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A364" s="2"/>
-      <c r="K364" s="2"/>
-    </row>
-    <row r="365" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A365" s="2"/>
-      <c r="K365" s="2"/>
-      <c r="Q365" s="3"/>
-      <c r="S365" s="3"/>
-    </row>
-    <row r="366" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="Q366" s="4"/>
-      <c r="S366" s="4"/>
-    </row>
-    <row r="367" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A367" s="2"/>
-      <c r="K367" s="2"/>
-      <c r="Q367" s="3"/>
-      <c r="S367" s="3"/>
-    </row>
-    <row r="368" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="Q368" s="3"/>
-      <c r="S368" s="3"/>
-    </row>
-    <row r="370" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A370" s="1"/>
-      <c r="B370" s="1"/>
-    </row>
-    <row r="372" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B372" s="2"/>
+    <row r="358" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A358" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>1</v>
+      </c>
+      <c r="B359">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>2</v>
+      </c>
+      <c r="B360" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>3</v>
+      </c>
+      <c r="B361" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>5</v>
+      </c>
+      <c r="B362" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>7</v>
+      </c>
+      <c r="B363" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>9</v>
+      </c>
+      <c r="B364" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>32</v>
+      </c>
+      <c r="B365" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A366" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>11</v>
+      </c>
+      <c r="B367" t="s">
+        <v>12</v>
+      </c>
+      <c r="C367" t="s">
+        <v>7</v>
+      </c>
+      <c r="D367" t="s">
+        <v>5</v>
+      </c>
+      <c r="E367" t="s">
+        <v>13</v>
+      </c>
+      <c r="F367" t="s">
+        <v>3</v>
+      </c>
+      <c r="G367" t="s">
+        <v>14</v>
+      </c>
+      <c r="H367" t="s">
+        <v>15</v>
+      </c>
+      <c r="I367" t="s">
+        <v>16</v>
+      </c>
+      <c r="J367" t="s">
+        <v>2</v>
+      </c>
+      <c r="K367" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A368" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B368">
+        <v>1</v>
+      </c>
+      <c r="C368" t="s">
+        <v>8</v>
+      </c>
+      <c r="D368" t="s">
+        <v>5</v>
+      </c>
+      <c r="E368" t="s">
+        <v>69</v>
+      </c>
+      <c r="F368" t="s">
+        <v>18</v>
+      </c>
+      <c r="J368" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K368" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="369" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>114</v>
+      </c>
+      <c r="B369">
+        <v>97.5</v>
+      </c>
+      <c r="C369" t="s">
+        <v>61</v>
+      </c>
+      <c r="D369" t="s">
+        <v>6</v>
+      </c>
+      <c r="E369" t="s">
+        <v>19</v>
+      </c>
+      <c r="F369" t="s">
+        <v>20</v>
+      </c>
+      <c r="G369">
+        <v>2</v>
+      </c>
+      <c r="H369">
+        <v>4.5798523780038014</v>
+      </c>
+      <c r="I369">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J369" t="s">
+        <v>115</v>
+      </c>
+      <c r="K369" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="370" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>85</v>
+      </c>
+      <c r="B370">
+        <v>3000</v>
+      </c>
+      <c r="C370" t="s">
+        <v>86</v>
+      </c>
+      <c r="D370" t="s">
+        <v>6</v>
+      </c>
+      <c r="E370" t="s">
+        <v>19</v>
+      </c>
+      <c r="F370" t="s">
+        <v>20</v>
+      </c>
+      <c r="G370">
+        <v>2</v>
+      </c>
+      <c r="H370">
+        <v>8.0063675676502459</v>
+      </c>
+      <c r="I370">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J370" t="s">
+        <v>87</v>
+      </c>
+      <c r="K370" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="371" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>88</v>
+      </c>
+      <c r="B371">
+        <v>52.5</v>
+      </c>
+      <c r="C371" t="s">
+        <v>8</v>
+      </c>
+      <c r="D371" t="s">
+        <v>6</v>
+      </c>
+      <c r="E371" t="s">
+        <v>19</v>
+      </c>
+      <c r="F371" t="s">
+        <v>20</v>
+      </c>
+      <c r="G371">
+        <v>2</v>
+      </c>
+      <c r="H371">
+        <v>3.9608131695975781</v>
+      </c>
+      <c r="I371">
+        <v>2.439508208471609E-2</v>
+      </c>
+      <c r="J371" t="s">
+        <v>89</v>
+      </c>
+      <c r="K371" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="372" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>90</v>
+      </c>
+      <c r="B372">
+        <v>4000</v>
+      </c>
+      <c r="C372" t="s">
+        <v>8</v>
+      </c>
+      <c r="D372" t="s">
+        <v>65</v>
+      </c>
+      <c r="E372" t="s">
+        <v>19</v>
+      </c>
+      <c r="F372" t="s">
+        <v>20</v>
+      </c>
+      <c r="G372">
+        <v>2</v>
+      </c>
+      <c r="H372">
+        <v>8.2940496401020276</v>
+      </c>
+      <c r="I372">
+        <v>0.3465735902799727</v>
+      </c>
+      <c r="J372" t="s">
+        <v>90</v>
+      </c>
+      <c r="K372" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="378" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A378" s="1"/>
@@ -7173,76 +7273,96 @@
       <c r="Q400" s="3"/>
       <c r="S400" s="3"/>
     </row>
-    <row r="402" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A402" s="1"/>
       <c r="B402" s="1"/>
     </row>
-    <row r="404" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B404" s="2"/>
     </row>
-    <row r="409" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A409" s="1"/>
-    </row>
-    <row r="411" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A411" s="2"/>
-      <c r="K411" s="2"/>
-    </row>
-    <row r="414" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A414" s="1"/>
-      <c r="B414" s="1"/>
-    </row>
-    <row r="416" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B416" s="2"/>
-    </row>
-    <row r="421" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A421" s="1"/>
-    </row>
-    <row r="424" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A424" s="2"/>
-      <c r="M424" s="2"/>
-    </row>
-    <row r="429" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A429" s="1"/>
-      <c r="B429" s="1"/>
-    </row>
-    <row r="431" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B431" s="2"/>
-    </row>
-    <row r="436" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A436" s="1"/>
-    </row>
-    <row r="438" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A438" s="2"/>
-      <c r="J438" s="2"/>
-    </row>
-    <row r="439" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A439" s="2"/>
-    </row>
-    <row r="440" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A410" s="1"/>
+    </row>
+    <row r="412" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A412" s="2"/>
+      <c r="K412" s="2"/>
+    </row>
+    <row r="413" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A413" s="2"/>
+      <c r="K413" s="2"/>
+      <c r="Q413" s="3"/>
+      <c r="S413" s="3"/>
+    </row>
+    <row r="414" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q414" s="4"/>
+      <c r="S414" s="4"/>
+    </row>
+    <row r="415" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A415" s="2"/>
+      <c r="K415" s="2"/>
+      <c r="Q415" s="3"/>
+      <c r="S415" s="3"/>
+    </row>
+    <row r="416" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q416" s="3"/>
+      <c r="S416" s="3"/>
+    </row>
+    <row r="418" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A418" s="1"/>
+      <c r="B418" s="1"/>
+    </row>
+    <row r="420" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B420" s="2"/>
+    </row>
+    <row r="425" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A425" s="1"/>
+    </row>
+    <row r="427" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A427" s="2"/>
+      <c r="K427" s="2"/>
+    </row>
+    <row r="430" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A430" s="1"/>
+      <c r="B430" s="1"/>
+    </row>
+    <row r="432" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B432" s="2"/>
+    </row>
+    <row r="437" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A437" s="1"/>
+    </row>
+    <row r="440" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A440" s="2"/>
-    </row>
-    <row r="441" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A441" s="2"/>
-    </row>
-    <row r="442" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A442" s="2"/>
-    </row>
-    <row r="445" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A445" s="2"/>
-    </row>
-    <row r="447" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A447" s="1"/>
-      <c r="B447" s="1"/>
-    </row>
-    <row r="449" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B449" s="2"/>
+      <c r="M440" s="2"/>
+    </row>
+    <row r="445" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A445" s="1"/>
+      <c r="B445" s="1"/>
+    </row>
+    <row r="447" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B447" s="2"/>
+    </row>
+    <row r="452" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A452" s="1"/>
     </row>
     <row r="454" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A454" s="1"/>
+      <c r="A454" s="2"/>
+      <c r="J454" s="2"/>
+    </row>
+    <row r="455" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A455" s="2"/>
     </row>
     <row r="456" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A456" s="2"/>
-      <c r="J456" s="2"/>
+    </row>
+    <row r="457" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A457" s="2"/>
+    </row>
+    <row r="458" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A458" s="2"/>
+    </row>
+    <row r="461" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A461" s="2"/>
     </row>
     <row r="463" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A463" s="1"/>
@@ -7272,53 +7392,67 @@
       <c r="A488" s="2"/>
       <c r="J488" s="2"/>
     </row>
-    <row r="492" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A492" s="1"/>
-      <c r="B492" s="1"/>
-    </row>
-    <row r="494" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B494" s="2"/>
-    </row>
-    <row r="499" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A499" s="1"/>
-    </row>
-    <row r="501" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A501" s="2"/>
-    </row>
-    <row r="510" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A510" s="1"/>
-      <c r="B510" s="1"/>
+    <row r="495" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A495" s="1"/>
+      <c r="B495" s="1"/>
+    </row>
+    <row r="497" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B497" s="2"/>
+    </row>
+    <row r="502" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A502" s="1"/>
+    </row>
+    <row r="504" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A504" s="2"/>
+      <c r="J504" s="2"/>
+    </row>
+    <row r="508" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A508" s="1"/>
+      <c r="B508" s="1"/>
+    </row>
+    <row r="510" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B510" s="2"/>
+    </row>
+    <row r="515" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A515" s="1"/>
     </row>
     <row r="517" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A517" s="1"/>
-    </row>
-    <row r="523" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A523" s="1"/>
-      <c r="B523" s="1"/>
-    </row>
-    <row r="530" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A530" s="1"/>
-    </row>
-    <row r="537" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A537" s="1"/>
-      <c r="B537" s="1"/>
+      <c r="A517" s="2"/>
+    </row>
+    <row r="526" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A526" s="1"/>
+      <c r="B526" s="1"/>
+    </row>
+    <row r="533" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A533" s="1"/>
     </row>
     <row r="539" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B539" s="2"/>
-    </row>
-    <row r="544" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A544" s="1"/>
-    </row>
-    <row r="546" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A546" s="2"/>
-      <c r="J546" s="2"/>
-    </row>
-    <row r="552" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A552" s="1"/>
-      <c r="B552" s="1"/>
-    </row>
-    <row r="559" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A559" s="1"/>
+      <c r="A539" s="1"/>
+      <c r="B539" s="1"/>
+    </row>
+    <row r="546" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A546" s="1"/>
+    </row>
+    <row r="553" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A553" s="1"/>
+      <c r="B553" s="1"/>
+    </row>
+    <row r="555" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B555" s="2"/>
+    </row>
+    <row r="560" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A560" s="1"/>
+    </row>
+    <row r="562" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A562" s="2"/>
+      <c r="J562" s="2"/>
+    </row>
+    <row r="568" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A568" s="1"/>
+      <c r="B568" s="1"/>
+    </row>
+    <row r="575" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A575" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Set the value separator to "," for solar PV efficiencies file
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-direct-air-capture.xlsx
+++ b/premise/data/additional_inventories/lci-direct-air-capture.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1"/>
 </workbook>
 </file>
 
@@ -378,13 +378,13 @@
     <t>assumptions: originally in RER. uses waste heat and electricity from grid, DAC unit located 1 km away from the synfuel plant, CO2 pressurized to 25 bar</t>
   </si>
   <si>
-    <t>Life cycle assessment of carbon dioxide removal technologies: a critical review. Tom Terlouw, Christian Bauer, Lorenzo Rosa and Marco Mazzotti. 2021. https://doi.org/10.1039/D0EE03757E</t>
-  </si>
-  <si>
     <t>Represents old infrastructures from ClimeWorks, might be outdated.</t>
   </si>
   <si>
     <t>Timofte A. A Life Cycle Assessment of the Climeworks technology for direct air capture of carbon dioxide, a semester project in the ecological systems design group. Institute of Environmental Engineering of ETH Zurich; 2013.</t>
+  </si>
+  <si>
+    <t>Life cycle assessment of direct air carbon capture and storage with low-carbon energy sources. Tom Terlouw, Karin Treyer, Christian Bauer and Marco Mazzotti. 2021 (in review). Energy &amp; Environmental Science</t>
   </si>
 </sst>
 </file>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="H242" sqref="H242"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="B228" sqref="B228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,7 +840,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1188,7 +1188,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1536,7 +1536,7 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1884,7 +1884,7 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2232,7 +2232,7 @@
         <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2580,7 +2580,7 @@
         <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2928,7 +2928,7 @@
         <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3276,7 +3276,7 @@
         <v>32</v>
       </c>
       <c r="B148" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3624,7 +3624,7 @@
         <v>32</v>
       </c>
       <c r="B168" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3972,7 +3972,7 @@
         <v>32</v>
       </c>
       <c r="B188" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -4320,7 +4320,7 @@
         <v>32</v>
       </c>
       <c r="B208" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -4668,7 +4668,7 @@
         <v>32</v>
       </c>
       <c r="B228" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -5024,7 +5024,7 @@
         <v>9</v>
       </c>
       <c r="B249" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.3">
@@ -5032,7 +5032,7 @@
         <v>32</v>
       </c>
       <c r="B250" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="251" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -5378,7 +5378,7 @@
         <v>9</v>
       </c>
       <c r="B268" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.3">
@@ -5386,7 +5386,7 @@
         <v>32</v>
       </c>
       <c r="B269" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="270" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -5683,7 +5683,7 @@
         <v>9</v>
       </c>
       <c r="B285" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.3">
@@ -5691,7 +5691,7 @@
         <v>32</v>
       </c>
       <c r="B286" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="287" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -5988,7 +5988,7 @@
         <v>9</v>
       </c>
       <c r="B302" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.3">
@@ -5996,7 +5996,7 @@
         <v>32</v>
       </c>
       <c r="B303" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="304" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -6188,7 +6188,7 @@
         <v>9</v>
       </c>
       <c r="B316" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.3">
@@ -6196,7 +6196,7 @@
         <v>32</v>
       </c>
       <c r="B317" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="318" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -6560,7 +6560,7 @@
         <v>9</v>
       </c>
       <c r="B335" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="336" spans="1:11" x14ac:dyDescent="0.3">
@@ -6568,7 +6568,7 @@
         <v>32</v>
       </c>
       <c r="B336" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="337" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -6760,7 +6760,7 @@
         <v>9</v>
       </c>
       <c r="B349" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="350" spans="1:11" x14ac:dyDescent="0.3">
@@ -6768,7 +6768,7 @@
         <v>32</v>
       </c>
       <c r="B350" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="351" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -6995,7 +6995,7 @@
         <v>9</v>
       </c>
       <c r="B364" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.3">
@@ -7003,7 +7003,7 @@
         <v>32</v>
       </c>
       <c r="B365" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="366" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Progress on fuels integration
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-direct-air-capture.xlsx
+++ b/premise/data/additional_inventories/lci-direct-air-capture.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="DAC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -180,9 +180,6 @@
     <t>sorbant</t>
   </si>
   <si>
-    <t>transport, freight, lorry &gt;32 metric ton, EURO6</t>
-  </si>
-  <si>
     <t>ton kilometer</t>
   </si>
   <si>
@@ -258,9 +255,6 @@
     <t>synthetic rubber</t>
   </si>
   <si>
-    <t>transport, freight, lorry 16-32 metric ton, EURO5</t>
-  </si>
-  <si>
     <t>computer production, desktop, without screen</t>
   </si>
   <si>
@@ -349,6 +343,12 @@
   </si>
   <si>
     <t>Life cycle assessment of direct air carbon capture and storage with low-carbon energy sources. Tom Terlouw, Karin Treyer, Christian Bauer and Marco Mazzotti. 2021 (in review). Energy &amp; Environmental Science</t>
+  </si>
+  <si>
+    <t>market for transport, freight, lorry, unspecified</t>
+  </si>
+  <si>
+    <t>transport, freight, lorry, unspecified</t>
   </si>
 </sst>
 </file>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,7 +796,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -804,7 +804,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -984,7 +984,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B17" s="6">
         <v>0.57799999999999996</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="B20" s="6">
         <v>7.4399999999999992E-5</v>
@@ -1068,21 +1068,21 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s">
         <v>20</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="6">
         <f>1/1000*1</f>
@@ -1095,16 +1095,16 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s">
         <v>20</v>
       </c>
       <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" t="s">
         <v>56</v>
-      </c>
-      <c r="I21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1160,7 +1160,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1168,7 +1168,7 @@
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1225,7 +1225,7 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F33" t="s">
         <v>18</v>
@@ -1234,12 +1234,12 @@
         <v>34</v>
       </c>
       <c r="K33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34">
         <v>1.09529E-7</v>
@@ -1266,12 +1266,12 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="K34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35">
         <v>1.09529E-7</v>
@@ -1298,12 +1298,12 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="K35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36">
         <v>1.09529E-7</v>
@@ -1330,12 +1330,12 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="K36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37">
         <v>1.09529E-7</v>
@@ -1362,12 +1362,12 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="K37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38">
         <v>1.09529E-7</v>
@@ -1394,12 +1394,12 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="K38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39">
         <v>1.09529E-7</v>
@@ -1426,12 +1426,12 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="K39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40">
         <v>1.09529E-7</v>
@@ -1458,7 +1458,7 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="K40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -1482,7 +1482,7 @@
         <v>2</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -1514,7 +1514,7 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -1522,7 +1522,7 @@
         <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1567,7 +1567,7 @@
     </row>
     <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1579,33 +1579,33 @@
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F52" t="s">
         <v>18</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53">
         <v>13000</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F53" t="s">
         <v>20</v>
@@ -1620,15 +1620,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K53" t="s">
         <v>70</v>
-      </c>
-      <c r="K53" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B54">
         <v>500</v>
@@ -1640,7 +1640,7 @@
         <v>6</v>
       </c>
       <c r="E54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
@@ -1655,27 +1655,27 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B55">
         <v>500</v>
       </c>
       <c r="C55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F55" t="s">
         <v>20</v>
@@ -1690,15 +1690,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56">
         <v>120</v>
@@ -1710,7 +1710,7 @@
         <v>6</v>
       </c>
       <c r="E56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F56" t="s">
         <v>20</v>
@@ -1725,15 +1725,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B57">
         <v>15000</v>
@@ -1742,10 +1742,10 @@
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F57" t="s">
         <v>20</v>
@@ -1760,10 +1760,10 @@
         <v>0.2126338677021721</v>
       </c>
       <c r="J57" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="K57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
@@ -1787,7 +1787,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
@@ -1819,7 +1819,7 @@
         <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
@@ -1827,7 +1827,7 @@
         <v>23</v>
       </c>
       <c r="B66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1872,7 +1872,7 @@
     </row>
     <row r="69" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1884,21 +1884,21 @@
         <v>5</v>
       </c>
       <c r="E69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F69" t="s">
         <v>18</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -1925,15 +1925,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J70" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B71">
         <v>50</v>
@@ -1960,15 +1960,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J71" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -1995,15 +1995,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B73">
         <v>80000</v>
@@ -2012,7 +2012,7 @@
         <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
@@ -2030,15 +2030,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J73" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2065,10 +2065,10 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J74" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2076,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
@@ -2092,7 +2092,7 @@
         <v>2</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
@@ -2124,7 +2124,7 @@
         <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
@@ -2132,7 +2132,7 @@
         <v>23</v>
       </c>
       <c r="B83" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2177,7 +2177,7 @@
     </row>
     <row r="86" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2189,21 +2189,21 @@
         <v>5</v>
       </c>
       <c r="E86" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F86" t="s">
         <v>18</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K86" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B87">
         <v>854</v>
@@ -2230,21 +2230,21 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K87" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B88">
         <v>454</v>
       </c>
       <c r="C88" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
@@ -2265,10 +2265,10 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J88" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K88" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2276,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
@@ -2292,7 +2292,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
@@ -2324,7 +2324,7 @@
         <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
@@ -2332,7 +2332,7 @@
         <v>23</v>
       </c>
       <c r="B97" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2377,7 +2377,7 @@
     </row>
     <row r="100" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2389,18 +2389,18 @@
         <v>5</v>
       </c>
       <c r="E100" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F100" t="s">
         <v>18</v>
       </c>
       <c r="K100" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B101">
         <v>9000</v>
@@ -2427,15 +2427,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J101" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K101" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B102">
         <v>3.54</v>
@@ -2462,21 +2462,21 @@
         <v>5.6664342653501683E-2</v>
       </c>
       <c r="J102" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K102" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B103">
         <v>1180</v>
       </c>
       <c r="C103" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D103" t="s">
         <v>6</v>
@@ -2497,21 +2497,21 @@
         <v>5.6664342653501683E-2</v>
       </c>
       <c r="J103" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K103" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B104">
         <v>1180</v>
       </c>
       <c r="C104" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D104" t="s">
         <v>6</v>
@@ -2532,15 +2532,15 @@
         <v>5.6664342653501683E-2</v>
       </c>
       <c r="J104" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K104" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B105">
         <v>1418</v>
@@ -2549,7 +2549,7 @@
         <v>37</v>
       </c>
       <c r="D105" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -2567,15 +2567,15 @@
         <v>5.6664342653501683E-2</v>
       </c>
       <c r="J105" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K105" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B106">
         <v>1000</v>
@@ -2584,7 +2584,7 @@
         <v>8</v>
       </c>
       <c r="D106" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -2602,15 +2602,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J106" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="K106" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B107">
         <v>118</v>
@@ -2619,7 +2619,7 @@
         <v>8</v>
       </c>
       <c r="D107" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E107" t="s">
         <v>19</v>
@@ -2637,10 +2637,10 @@
         <v>5.6664342653501683E-2</v>
       </c>
       <c r="J107" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="K107" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
@@ -2664,7 +2664,7 @@
         <v>2</v>
       </c>
       <c r="B111" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
@@ -2696,7 +2696,7 @@
         <v>9</v>
       </c>
       <c r="B115" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.3">
@@ -2704,7 +2704,7 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2749,7 +2749,7 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -2761,27 +2761,27 @@
         <v>5</v>
       </c>
       <c r="E119" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F119" t="s">
         <v>18</v>
       </c>
       <c r="J119" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K119" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B120">
         <v>2000</v>
       </c>
       <c r="C120" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D120" t="s">
         <v>6</v>
@@ -2802,15 +2802,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J120" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K120" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B121">
         <v>2000</v>
@@ -2819,7 +2819,7 @@
         <v>8</v>
       </c>
       <c r="D121" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E121" t="s">
         <v>19</v>
@@ -2837,10 +2837,10 @@
         <v>0.3465735902799727</v>
       </c>
       <c r="J121" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="K121" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="123" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2848,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.3">
@@ -2864,7 +2864,7 @@
         <v>2</v>
       </c>
       <c r="B125" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.3">
@@ -2896,7 +2896,7 @@
         <v>9</v>
       </c>
       <c r="B129" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.3">
@@ -2904,7 +2904,7 @@
         <v>23</v>
       </c>
       <c r="B130" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="131" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2949,7 +2949,7 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2961,21 +2961,21 @@
         <v>5</v>
       </c>
       <c r="E133" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F133" t="s">
         <v>18</v>
       </c>
       <c r="J133" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K133" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B134">
         <v>0.17</v>
@@ -3002,15 +3002,15 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="J134" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K134" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B135">
         <v>125</v>
@@ -3037,15 +3037,15 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="J135" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K135" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B136">
         <v>818</v>
@@ -3072,10 +3072,10 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J136" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K136" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="138" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -3083,7 +3083,7 @@
         <v>0</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.3">
@@ -3099,7 +3099,7 @@
         <v>2</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.3">
@@ -3131,7 +3131,7 @@
         <v>9</v>
       </c>
       <c r="B144" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.3">
@@ -3139,7 +3139,7 @@
         <v>23</v>
       </c>
       <c r="B145" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="146" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -3184,7 +3184,7 @@
     </row>
     <row r="148" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -3196,21 +3196,21 @@
         <v>5</v>
       </c>
       <c r="E148" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F148" t="s">
         <v>18</v>
       </c>
       <c r="J148" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K148" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B149">
         <v>97.5</v>
@@ -3237,21 +3237,21 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J149" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K149" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B150">
         <v>3000</v>
       </c>
       <c r="C150" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D150" t="s">
         <v>6</v>
@@ -3272,15 +3272,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J150" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K150" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B151">
         <v>52.5</v>
@@ -3307,15 +3307,15 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="J151" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K151" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B152">
         <v>4000</v>
@@ -3324,7 +3324,7 @@
         <v>8</v>
       </c>
       <c r="D152" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E152" t="s">
         <v>19</v>
@@ -3342,10 +3342,10 @@
         <v>0.3465735902799727</v>
       </c>
       <c r="J152" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="K152" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="158" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Clear cache with version change Add IMAGE variables Add IMAGE scenarios Fix DAC LCI Update mapping_overview.xlsx Update docs
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-direct-air-capture.xlsx
+++ b/premise/data/additional_inventories/lci-direct-air-capture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57582260-1A4D-C64C-8C47-4E075BFF7FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFA78BA-230C-2749-9EF1-451145B58035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,6 @@
     <t>36% PEI</t>
   </si>
   <si>
-    <t>Synthesized by impregnate amines polyethylenimine (PEI) on solid silica gel. The LCI of amine-based silica is collected from literature and based on the composition that 1 kg amine-based silica requires of 0.64kg silica
-gel and 0.36 kg PEI.</t>
-  </si>
-  <si>
     <t>carbon dioxide compression, transport and storage</t>
   </si>
   <si>
@@ -593,17 +589,22 @@
   </si>
   <si>
     <t>operational</t>
+  </si>
+  <si>
+    <t>Synthesized by impregnate amines polyethylenimine (PEI) on solid silica gel. The LCI of amine-based silica is collected from literature and based on the composition that 1 kg amine-based silica requires of 0.64kg silica
+gel and 0.36 kg PEI. Inputs of ethanol and diethyl ether are reduced by 95% to account for recovery.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -686,7 +687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -703,6 +704,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1020,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34:G42"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1219,7 +1221,7 @@
         <v>3.4369999999999998</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -1231,12 +1233,12 @@
         <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17">
         <v>4.0000000000000001E-3</v>
@@ -1251,15 +1253,15 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B18">
         <v>3.5000000000000001E-3</v>
@@ -1274,10 +1276,10 @@
         <v>16</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1300,7 +1302,7 @@
         <v>83</v>
       </c>
       <c r="H19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1311,7 +1313,7 @@
         <v>6.28</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
@@ -1320,10 +1322,10 @@
         <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1343,7 +1345,7 @@
         <v>21</v>
       </c>
       <c r="H21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1363,7 +1365,7 @@
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1371,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1463,7 +1465,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1537,7 +1539,7 @@
         <v>3.4369999999999998</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1549,12 +1551,12 @@
         <v>34</v>
       </c>
       <c r="H37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B38">
         <v>4.0000000000000001E-3</v>
@@ -1569,15 +1571,15 @@
         <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B39">
         <v>3.5000000000000001E-3</v>
@@ -1592,10 +1594,10 @@
         <v>16</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1618,7 +1620,7 @@
         <v>83</v>
       </c>
       <c r="H40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1629,7 +1631,7 @@
         <v>6.28</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D41" t="s">
         <v>24</v>
@@ -1638,15 +1640,15 @@
         <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1661,10 +1663,10 @@
         <v>16</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1684,7 +1686,7 @@
         <v>21</v>
       </c>
       <c r="H43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1704,7 +1706,7 @@
         <v>21</v>
       </c>
       <c r="H44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2215,7 +2217,7 @@
         <v>16</v>
       </c>
       <c r="G73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H73" t="s">
         <v>65</v>
@@ -2348,7 +2350,7 @@
         <v>-760000000</v>
       </c>
       <c r="C86" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
@@ -2357,7 +2359,7 @@
         <v>16</v>
       </c>
       <c r="G86" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H86" s="12"/>
       <c r="Q86" s="4"/>
@@ -2380,7 +2382,7 @@
         <v>16</v>
       </c>
       <c r="G87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H87" s="12"/>
       <c r="Q87" s="3"/>
@@ -2403,7 +2405,7 @@
         <v>16</v>
       </c>
       <c r="G88" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H88" s="12"/>
       <c r="Q88" s="3"/>
@@ -2426,7 +2428,7 @@
         <v>16</v>
       </c>
       <c r="G89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
@@ -2448,7 +2450,7 @@
         <v>16</v>
       </c>
       <c r="G90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H90" s="12"/>
     </row>
@@ -2469,7 +2471,7 @@
         <v>16</v>
       </c>
       <c r="G91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H91" s="12"/>
     </row>
@@ -2490,7 +2492,7 @@
         <v>16</v>
       </c>
       <c r="G92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H92" s="12"/>
     </row>
@@ -2523,7 +2525,7 @@
         <v>-80000000</v>
       </c>
       <c r="C94" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -2532,7 +2534,7 @@
         <v>16</v>
       </c>
       <c r="G94" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H94" s="12"/>
     </row>
@@ -2553,7 +2555,7 @@
         <v>16</v>
       </c>
       <c r="G95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H95" s="12"/>
     </row>
@@ -2562,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -2610,7 +2612,7 @@
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -2654,7 +2656,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2692,12 +2694,12 @@
         <v>86</v>
       </c>
       <c r="H108" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B109">
         <f>1/(100000000*20)</f>
@@ -2721,7 +2723,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="B110">
         <f>-1/(100000000*20)</f>
@@ -2763,7 +2765,7 @@
         <v>83</v>
       </c>
       <c r="H111" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -2774,7 +2776,7 @@
         <v>5.4</v>
       </c>
       <c r="C112" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D112" t="s">
         <v>24</v>
@@ -2783,10 +2785,10 @@
         <v>16</v>
       </c>
       <c r="G112" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H112" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -2806,7 +2808,7 @@
         <v>21</v>
       </c>
       <c r="H113" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -2826,7 +2828,7 @@
         <v>21</v>
       </c>
       <c r="H114" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2834,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -2882,7 +2884,7 @@
         <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -2926,7 +2928,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2964,12 +2966,12 @@
         <v>86</v>
       </c>
       <c r="H127" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B128">
         <f>1/(100000000*20)</f>
@@ -2993,7 +2995,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="B129">
         <f>-1/(100000000*20)</f>
@@ -3035,7 +3037,7 @@
         <v>83</v>
       </c>
       <c r="H130" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -3046,7 +3048,7 @@
         <v>5.4</v>
       </c>
       <c r="C131" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D131" t="s">
         <v>24</v>
@@ -3055,15 +3057,15 @@
         <v>16</v>
       </c>
       <c r="G131" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H131" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -3078,10 +3080,10 @@
         <v>16</v>
       </c>
       <c r="G132" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H132" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -3101,7 +3103,7 @@
         <v>21</v>
       </c>
       <c r="H133" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -3121,7 +3123,7 @@
         <v>21</v>
       </c>
       <c r="H134" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3129,7 +3131,7 @@
         <v>0</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -3177,7 +3179,7 @@
         <v>9</v>
       </c>
       <c r="B142" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -3221,7 +3223,7 @@
     </row>
     <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -3259,12 +3261,12 @@
         <v>53</v>
       </c>
       <c r="H147" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B148">
         <v>942000</v>
@@ -3282,7 +3284,7 @@
         <v>35</v>
       </c>
       <c r="H148" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -3305,12 +3307,12 @@
         <v>53</v>
       </c>
       <c r="H149" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B150">
         <v>548000.00000000012</v>
@@ -3328,7 +3330,7 @@
         <v>35</v>
       </c>
       <c r="H150" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -3351,12 +3353,12 @@
         <v>32</v>
       </c>
       <c r="H151" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B152">
         <v>16000</v>
@@ -3371,10 +3373,10 @@
         <v>16</v>
       </c>
       <c r="G152" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H152" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -3394,10 +3396,10 @@
         <v>16</v>
       </c>
       <c r="G153" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H153" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -3420,12 +3422,12 @@
         <v>54</v>
       </c>
       <c r="H154" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B155">
         <v>10000</v>
@@ -3440,15 +3442,15 @@
         <v>16</v>
       </c>
       <c r="G155" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H155" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B156">
         <v>12000</v>
@@ -3463,15 +3465,15 @@
         <v>16</v>
       </c>
       <c r="G156" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H156" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B157">
         <v>10000</v>
@@ -3486,10 +3488,10 @@
         <v>16</v>
       </c>
       <c r="G157" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H157" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -3512,12 +3514,12 @@
         <v>64</v>
       </c>
       <c r="H158" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B159">
         <v>10000</v>
@@ -3532,10 +3534,10 @@
         <v>16</v>
       </c>
       <c r="G159" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H159" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -3558,7 +3560,7 @@
         <v>54</v>
       </c>
       <c r="H160" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -3581,12 +3583,12 @@
         <v>32</v>
       </c>
       <c r="H161" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B162">
         <v>94000</v>
@@ -3601,15 +3603,15 @@
         <v>16</v>
       </c>
       <c r="G162" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H162" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B163">
         <v>10000</v>
@@ -3624,15 +3626,15 @@
         <v>16</v>
       </c>
       <c r="G163" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H163" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B164">
         <v>10000</v>
@@ -3647,10 +3649,10 @@
         <v>16</v>
       </c>
       <c r="G164" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H164" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -3673,7 +3675,7 @@
         <v>54</v>
       </c>
       <c r="H165" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
@@ -3696,7 +3698,7 @@
         <v>32</v>
       </c>
       <c r="H166" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
@@ -3707,7 +3709,7 @@
         <v>0</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -3755,7 +3757,7 @@
         <v>9</v>
       </c>
       <c r="B174" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -3799,7 +3801,7 @@
     </row>
     <row r="178" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B178">
         <v>-1</v>
@@ -3825,7 +3827,7 @@
         <v>-29400000</v>
       </c>
       <c r="C179" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D179" t="s">
         <v>6</v>
@@ -3834,7 +3836,7 @@
         <v>16</v>
       </c>
       <c r="G179" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q179" s="4"/>
       <c r="S179" s="4"/>
@@ -3856,7 +3858,7 @@
         <v>16</v>
       </c>
       <c r="G180" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q180" s="3"/>
       <c r="S180" s="3"/>
@@ -3878,7 +3880,7 @@
         <v>16</v>
       </c>
       <c r="G181" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q181" s="3"/>
       <c r="S181" s="3"/>
@@ -3911,7 +3913,7 @@
         <v>-6000000</v>
       </c>
       <c r="C183" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D183" t="s">
         <v>6</v>
@@ -3920,18 +3922,18 @@
         <v>16</v>
       </c>
       <c r="G183" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="184" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B184">
         <v>-20000</v>
       </c>
       <c r="C184" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D184" t="s">
         <v>6</v>
@@ -3940,18 +3942,18 @@
         <v>16</v>
       </c>
       <c r="G184" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="185" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B185">
         <v>-26000</v>
       </c>
       <c r="C185" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D185" t="s">
         <v>6</v>
@@ -3960,7 +3962,7 @@
         <v>16</v>
       </c>
       <c r="G185" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="186" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -4019,7 +4021,7 @@
         <v>9</v>
       </c>
       <c r="B193" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
     </row>
     <row r="194" spans="1:19" x14ac:dyDescent="0.2">
@@ -4195,7 +4197,7 @@
         <v>16</v>
       </c>
       <c r="G202" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H202" t="s">
         <v>104</v>
@@ -4204,7 +4206,7 @@
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B203">
         <v>4.1999999999999998E-5</v>
@@ -4239,7 +4241,7 @@
         <v>16</v>
       </c>
       <c r="G204" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H204" t="s">
         <v>105</v>
@@ -4285,7 +4287,7 @@
         <v>16</v>
       </c>
       <c r="G206" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H206" t="s">
         <v>105</v>
@@ -4308,7 +4310,7 @@
         <v>16</v>
       </c>
       <c r="G207" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H207" t="s">
         <v>105</v>
@@ -4319,7 +4321,8 @@
         <v>101</v>
       </c>
       <c r="B208">
-        <v>1.24</v>
+        <f>1.24*0.05</f>
+        <v>6.2E-2</v>
       </c>
       <c r="C208" t="s">
         <v>18</v>
@@ -4331,7 +4334,7 @@
         <v>16</v>
       </c>
       <c r="G208" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H208" t="s">
         <v>105</v>
@@ -4341,8 +4344,9 @@
       <c r="A209" t="s">
         <v>102</v>
       </c>
-      <c r="B209" s="2">
-        <v>14.84</v>
+      <c r="B209" s="14">
+        <f>0.36*(AVERAGE(33.94,48.48))*(1-0.97)</f>
+        <v>0.44506800000000035</v>
       </c>
       <c r="C209" t="s">
         <v>28</v>
@@ -4354,7 +4358,7 @@
         <v>16</v>
       </c>
       <c r="G209" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H209" t="s">
         <v>105</v>
@@ -4414,7 +4418,7 @@
         <v>2.69</v>
       </c>
       <c r="C212" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D212" t="s">
         <v>24</v>
@@ -4446,7 +4450,7 @@
         <v>16</v>
       </c>
       <c r="G213" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H213" t="s">
         <v>105</v>
@@ -4460,7 +4464,7 @@
         <v>-0.54</v>
       </c>
       <c r="C214" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D214" t="s">
         <v>6</v>
@@ -4469,7 +4473,7 @@
         <v>16</v>
       </c>
       <c r="G214" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H214" t="s">
         <v>105</v>
@@ -4507,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.2">
@@ -4523,7 +4527,7 @@
         <v>2</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
@@ -4555,7 +4559,7 @@
         <v>9</v>
       </c>
       <c r="B223" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.2">
@@ -4599,7 +4603,7 @@
     </row>
     <row r="227" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -4614,7 +4618,7 @@
         <v>15</v>
       </c>
       <c r="G227" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.2">
@@ -4637,12 +4641,12 @@
         <v>53</v>
       </c>
       <c r="H228" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B229">
         <v>1.0000000000000001E-7</v>
@@ -4657,10 +4661,10 @@
         <v>16</v>
       </c>
       <c r="G229" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H229" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.2">
@@ -4683,12 +4687,12 @@
         <v>32</v>
       </c>
       <c r="H230" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B231">
         <v>2.9999999999999999E-7</v>
@@ -4703,15 +4707,15 @@
         <v>16</v>
       </c>
       <c r="G231" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H231" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B232">
         <v>3.1999999999999999E-5</v>
@@ -4726,10 +4730,10 @@
         <v>16</v>
       </c>
       <c r="G232" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H232" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -4752,12 +4756,12 @@
         <v>83</v>
       </c>
       <c r="H233" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="234" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B234">
         <v>1.0400000000000001E-3</v>
@@ -4772,16 +4776,16 @@
         <v>16</v>
       </c>
       <c r="G234" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H234" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J234" s="2"/>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B235">
         <v>1.3000000000000002E-4</v>
@@ -4799,12 +4803,12 @@
         <v>35</v>
       </c>
       <c r="H235" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B236">
         <v>1.3000000000000002E-4</v>
@@ -4819,15 +4823,15 @@
         <v>16</v>
       </c>
       <c r="G236" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H236" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B237">
         <v>1.1999999999999999E-6</v>
@@ -4842,15 +4846,15 @@
         <v>16</v>
       </c>
       <c r="G237" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H237" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B238">
         <v>2.5000000000000002E-6</v>
@@ -4865,15 +4869,15 @@
         <v>16</v>
       </c>
       <c r="G238" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H238" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B239">
         <v>1.8E-3</v>
@@ -4888,10 +4892,10 @@
         <v>16</v>
       </c>
       <c r="G239" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H239" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.2">
@@ -4914,12 +4918,12 @@
         <v>38</v>
       </c>
       <c r="H240" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B241" s="6">
         <v>8.2000000000000001E-11</v>
@@ -4928,21 +4932,21 @@
         <v>18</v>
       </c>
       <c r="D241" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F241" t="s">
         <v>16</v>
       </c>
       <c r="G241" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H241" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B242">
         <v>3.3E-3</v>
@@ -4957,10 +4961,10 @@
         <v>16</v>
       </c>
       <c r="G242" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H242" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="243" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4980,10 +4984,10 @@
         <v>16</v>
       </c>
       <c r="G243" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H243" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.2">
@@ -5006,7 +5010,7 @@
         <v>32</v>
       </c>
       <c r="H244" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.2">
@@ -5029,12 +5033,12 @@
         <v>53</v>
       </c>
       <c r="H245" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B246">
         <v>1.9E-6</v>
@@ -5049,10 +5053,10 @@
         <v>16</v>
       </c>
       <c r="G246" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H246" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
@@ -5075,7 +5079,7 @@
         <v>38</v>
       </c>
       <c r="H247" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.2">
@@ -5098,7 +5102,7 @@
         <v>83</v>
       </c>
       <c r="H248" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.2">
@@ -5109,7 +5113,7 @@
         <v>-4.4000000000000003E-3</v>
       </c>
       <c r="C249" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D249" s="10" t="s">
         <v>6</v>
@@ -5118,7 +5122,7 @@
         <v>16</v>
       </c>
       <c r="G249" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H249" t="s">
         <v>81</v>
@@ -5141,7 +5145,7 @@
         <v>16</v>
       </c>
       <c r="G250" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H250" t="s">
         <v>81</v>
@@ -5150,13 +5154,13 @@
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B251">
         <v>-1.9999999999999999E-6</v>
       </c>
       <c r="C251" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D251" s="10" t="s">
         <v>6</v>
@@ -5165,7 +5169,7 @@
         <v>16</v>
       </c>
       <c r="G251" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H251" t="s">
         <v>81</v>
@@ -5173,7 +5177,7 @@
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B252">
         <v>-2.7999999999999999E-6</v>
@@ -5188,7 +5192,7 @@
         <v>16</v>
       </c>
       <c r="G252" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H252" t="s">
         <v>81</v>
@@ -5196,13 +5200,13 @@
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B253">
         <v>-1.1999999999999999E-6</v>
       </c>
       <c r="C253" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D253" s="10" t="s">
         <v>6</v>
@@ -5211,7 +5215,7 @@
         <v>16</v>
       </c>
       <c r="G253" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H253" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Revert "Clear cache with version change"
This reverts commit 71949ab8a10aa90fd83b87bf2e59e3697b8f3f16.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-direct-air-capture.xlsx
+++ b/premise/data/additional_inventories/lci-direct-air-capture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFA78BA-230C-2749-9EF1-451145B58035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57582260-1A4D-C64C-8C47-4E075BFF7FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,6 +356,10 @@
     <t>36% PEI</t>
   </si>
   <si>
+    <t>Synthesized by impregnate amines polyethylenimine (PEI) on solid silica gel. The LCI of amine-based silica is collected from literature and based on the composition that 1 kg amine-based silica requires of 0.64kg silica
+gel and 0.36 kg PEI.</t>
+  </si>
+  <si>
     <t>carbon dioxide compression, transport and storage</t>
   </si>
   <si>
@@ -589,22 +593,17 @@
   </si>
   <si>
     <t>operational</t>
-  </si>
-  <si>
-    <t>Synthesized by impregnate amines polyethylenimine (PEI) on solid silica gel. The LCI of amine-based silica is collected from literature and based on the composition that 1 kg amine-based silica requires of 0.64kg silica
-gel and 0.36 kg PEI. Inputs of ethanol and diethyl ether are reduced by 95% to account for recovery.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -687,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -704,7 +703,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1022,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="B209" sqref="B209"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1221,7 +1219,7 @@
         <v>3.4369999999999998</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -1233,12 +1231,12 @@
         <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B17">
         <v>4.0000000000000001E-3</v>
@@ -1253,15 +1251,15 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B18">
         <v>3.5000000000000001E-3</v>
@@ -1276,10 +1274,10 @@
         <v>16</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1302,7 +1300,7 @@
         <v>83</v>
       </c>
       <c r="H19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1313,7 +1311,7 @@
         <v>6.28</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
@@ -1322,10 +1320,10 @@
         <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1345,7 +1343,7 @@
         <v>21</v>
       </c>
       <c r="H21" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1365,7 +1363,7 @@
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1373,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1465,7 +1463,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1539,7 +1537,7 @@
         <v>3.4369999999999998</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1551,12 +1549,12 @@
         <v>34</v>
       </c>
       <c r="H37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B38">
         <v>4.0000000000000001E-3</v>
@@ -1571,15 +1569,15 @@
         <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H38" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B39">
         <v>3.5000000000000001E-3</v>
@@ -1594,10 +1592,10 @@
         <v>16</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1620,7 +1618,7 @@
         <v>83</v>
       </c>
       <c r="H40" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1631,7 +1629,7 @@
         <v>6.28</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D41" t="s">
         <v>24</v>
@@ -1640,15 +1638,15 @@
         <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H41" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1663,10 +1661,10 @@
         <v>16</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H42" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1686,7 +1684,7 @@
         <v>21</v>
       </c>
       <c r="H43" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1706,7 +1704,7 @@
         <v>21</v>
       </c>
       <c r="H44" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2217,7 +2215,7 @@
         <v>16</v>
       </c>
       <c r="G73" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H73" t="s">
         <v>65</v>
@@ -2350,7 +2348,7 @@
         <v>-760000000</v>
       </c>
       <c r="C86" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
@@ -2359,7 +2357,7 @@
         <v>16</v>
       </c>
       <c r="G86" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H86" s="12"/>
       <c r="Q86" s="4"/>
@@ -2382,7 +2380,7 @@
         <v>16</v>
       </c>
       <c r="G87" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H87" s="12"/>
       <c r="Q87" s="3"/>
@@ -2405,7 +2403,7 @@
         <v>16</v>
       </c>
       <c r="G88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H88" s="12"/>
       <c r="Q88" s="3"/>
@@ -2428,7 +2426,7 @@
         <v>16</v>
       </c>
       <c r="G89" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
@@ -2450,7 +2448,7 @@
         <v>16</v>
       </c>
       <c r="G90" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H90" s="12"/>
     </row>
@@ -2471,7 +2469,7 @@
         <v>16</v>
       </c>
       <c r="G91" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H91" s="12"/>
     </row>
@@ -2492,7 +2490,7 @@
         <v>16</v>
       </c>
       <c r="G92" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H92" s="12"/>
     </row>
@@ -2525,7 +2523,7 @@
         <v>-80000000</v>
       </c>
       <c r="C94" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -2534,7 +2532,7 @@
         <v>16</v>
       </c>
       <c r="G94" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H94" s="12"/>
     </row>
@@ -2555,7 +2553,7 @@
         <v>16</v>
       </c>
       <c r="G95" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H95" s="12"/>
     </row>
@@ -2564,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -2612,7 +2610,7 @@
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -2656,7 +2654,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2694,12 +2692,12 @@
         <v>86</v>
       </c>
       <c r="H108" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B109">
         <f>1/(100000000*20)</f>
@@ -2723,7 +2721,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="B110">
         <f>-1/(100000000*20)</f>
@@ -2765,7 +2763,7 @@
         <v>83</v>
       </c>
       <c r="H111" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -2776,7 +2774,7 @@
         <v>5.4</v>
       </c>
       <c r="C112" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D112" t="s">
         <v>24</v>
@@ -2785,10 +2783,10 @@
         <v>16</v>
       </c>
       <c r="G112" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H112" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -2808,7 +2806,7 @@
         <v>21</v>
       </c>
       <c r="H113" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -2828,7 +2826,7 @@
         <v>21</v>
       </c>
       <c r="H114" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2836,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -2884,7 +2882,7 @@
         <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -2928,7 +2926,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2966,12 +2964,12 @@
         <v>86</v>
       </c>
       <c r="H127" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B128">
         <f>1/(100000000*20)</f>
@@ -2995,7 +2993,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="B129">
         <f>-1/(100000000*20)</f>
@@ -3037,7 +3035,7 @@
         <v>83</v>
       </c>
       <c r="H130" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -3048,7 +3046,7 @@
         <v>5.4</v>
       </c>
       <c r="C131" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D131" t="s">
         <v>24</v>
@@ -3057,15 +3055,15 @@
         <v>16</v>
       </c>
       <c r="G131" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H131" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -3080,10 +3078,10 @@
         <v>16</v>
       </c>
       <c r="G132" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H132" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -3103,7 +3101,7 @@
         <v>21</v>
       </c>
       <c r="H133" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -3123,7 +3121,7 @@
         <v>21</v>
       </c>
       <c r="H134" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3131,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -3179,7 +3177,7 @@
         <v>9</v>
       </c>
       <c r="B142" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -3223,7 +3221,7 @@
     </row>
     <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -3261,12 +3259,12 @@
         <v>53</v>
       </c>
       <c r="H147" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B148">
         <v>942000</v>
@@ -3284,7 +3282,7 @@
         <v>35</v>
       </c>
       <c r="H148" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -3307,12 +3305,12 @@
         <v>53</v>
       </c>
       <c r="H149" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B150">
         <v>548000.00000000012</v>
@@ -3330,7 +3328,7 @@
         <v>35</v>
       </c>
       <c r="H150" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -3353,12 +3351,12 @@
         <v>32</v>
       </c>
       <c r="H151" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B152">
         <v>16000</v>
@@ -3373,10 +3371,10 @@
         <v>16</v>
       </c>
       <c r="G152" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H152" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -3396,10 +3394,10 @@
         <v>16</v>
       </c>
       <c r="G153" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H153" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -3422,12 +3420,12 @@
         <v>54</v>
       </c>
       <c r="H154" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B155">
         <v>10000</v>
@@ -3442,15 +3440,15 @@
         <v>16</v>
       </c>
       <c r="G155" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H155" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B156">
         <v>12000</v>
@@ -3465,15 +3463,15 @@
         <v>16</v>
       </c>
       <c r="G156" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H156" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B157">
         <v>10000</v>
@@ -3488,10 +3486,10 @@
         <v>16</v>
       </c>
       <c r="G157" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H157" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -3514,12 +3512,12 @@
         <v>64</v>
       </c>
       <c r="H158" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B159">
         <v>10000</v>
@@ -3534,10 +3532,10 @@
         <v>16</v>
       </c>
       <c r="G159" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H159" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -3560,7 +3558,7 @@
         <v>54</v>
       </c>
       <c r="H160" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -3583,12 +3581,12 @@
         <v>32</v>
       </c>
       <c r="H161" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B162">
         <v>94000</v>
@@ -3603,15 +3601,15 @@
         <v>16</v>
       </c>
       <c r="G162" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H162" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B163">
         <v>10000</v>
@@ -3626,15 +3624,15 @@
         <v>16</v>
       </c>
       <c r="G163" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H163" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B164">
         <v>10000</v>
@@ -3649,10 +3647,10 @@
         <v>16</v>
       </c>
       <c r="G164" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H164" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -3675,7 +3673,7 @@
         <v>54</v>
       </c>
       <c r="H165" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
@@ -3698,7 +3696,7 @@
         <v>32</v>
       </c>
       <c r="H166" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
@@ -3709,7 +3707,7 @@
         <v>0</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -3757,7 +3755,7 @@
         <v>9</v>
       </c>
       <c r="B174" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -3801,7 +3799,7 @@
     </row>
     <row r="178" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B178">
         <v>-1</v>
@@ -3827,7 +3825,7 @@
         <v>-29400000</v>
       </c>
       <c r="C179" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D179" t="s">
         <v>6</v>
@@ -3836,7 +3834,7 @@
         <v>16</v>
       </c>
       <c r="G179" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Q179" s="4"/>
       <c r="S179" s="4"/>
@@ -3858,7 +3856,7 @@
         <v>16</v>
       </c>
       <c r="G180" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Q180" s="3"/>
       <c r="S180" s="3"/>
@@ -3880,7 +3878,7 @@
         <v>16</v>
       </c>
       <c r="G181" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Q181" s="3"/>
       <c r="S181" s="3"/>
@@ -3913,7 +3911,7 @@
         <v>-6000000</v>
       </c>
       <c r="C183" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D183" t="s">
         <v>6</v>
@@ -3922,18 +3920,18 @@
         <v>16</v>
       </c>
       <c r="G183" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="184" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B184">
         <v>-20000</v>
       </c>
       <c r="C184" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D184" t="s">
         <v>6</v>
@@ -3942,18 +3940,18 @@
         <v>16</v>
       </c>
       <c r="G184" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="185" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B185">
         <v>-26000</v>
       </c>
       <c r="C185" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D185" t="s">
         <v>6</v>
@@ -3962,7 +3960,7 @@
         <v>16</v>
       </c>
       <c r="G185" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="186" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -4021,7 +4019,7 @@
         <v>9</v>
       </c>
       <c r="B193" t="s">
-        <v>184</v>
+        <v>106</v>
       </c>
     </row>
     <row r="194" spans="1:19" x14ac:dyDescent="0.2">
@@ -4197,7 +4195,7 @@
         <v>16</v>
       </c>
       <c r="G202" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H202" t="s">
         <v>104</v>
@@ -4206,7 +4204,7 @@
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B203">
         <v>4.1999999999999998E-5</v>
@@ -4241,7 +4239,7 @@
         <v>16</v>
       </c>
       <c r="G204" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H204" t="s">
         <v>105</v>
@@ -4287,7 +4285,7 @@
         <v>16</v>
       </c>
       <c r="G206" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H206" t="s">
         <v>105</v>
@@ -4310,7 +4308,7 @@
         <v>16</v>
       </c>
       <c r="G207" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H207" t="s">
         <v>105</v>
@@ -4321,8 +4319,7 @@
         <v>101</v>
       </c>
       <c r="B208">
-        <f>1.24*0.05</f>
-        <v>6.2E-2</v>
+        <v>1.24</v>
       </c>
       <c r="C208" t="s">
         <v>18</v>
@@ -4334,7 +4331,7 @@
         <v>16</v>
       </c>
       <c r="G208" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H208" t="s">
         <v>105</v>
@@ -4344,9 +4341,8 @@
       <c r="A209" t="s">
         <v>102</v>
       </c>
-      <c r="B209" s="14">
-        <f>0.36*(AVERAGE(33.94,48.48))*(1-0.97)</f>
-        <v>0.44506800000000035</v>
+      <c r="B209" s="2">
+        <v>14.84</v>
       </c>
       <c r="C209" t="s">
         <v>28</v>
@@ -4358,7 +4354,7 @@
         <v>16</v>
       </c>
       <c r="G209" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H209" t="s">
         <v>105</v>
@@ -4418,7 +4414,7 @@
         <v>2.69</v>
       </c>
       <c r="C212" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D212" t="s">
         <v>24</v>
@@ -4450,7 +4446,7 @@
         <v>16</v>
       </c>
       <c r="G213" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H213" t="s">
         <v>105</v>
@@ -4464,7 +4460,7 @@
         <v>-0.54</v>
       </c>
       <c r="C214" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D214" t="s">
         <v>6</v>
@@ -4473,7 +4469,7 @@
         <v>16</v>
       </c>
       <c r="G214" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H214" t="s">
         <v>105</v>
@@ -4511,7 +4507,7 @@
         <v>0</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.2">
@@ -4527,7 +4523,7 @@
         <v>2</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
@@ -4559,7 +4555,7 @@
         <v>9</v>
       </c>
       <c r="B223" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.2">
@@ -4603,7 +4599,7 @@
     </row>
     <row r="227" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -4618,7 +4614,7 @@
         <v>15</v>
       </c>
       <c r="G227" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.2">
@@ -4641,12 +4637,12 @@
         <v>53</v>
       </c>
       <c r="H228" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B229">
         <v>1.0000000000000001E-7</v>
@@ -4661,10 +4657,10 @@
         <v>16</v>
       </c>
       <c r="G229" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H229" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.2">
@@ -4687,12 +4683,12 @@
         <v>32</v>
       </c>
       <c r="H230" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B231">
         <v>2.9999999999999999E-7</v>
@@ -4707,15 +4703,15 @@
         <v>16</v>
       </c>
       <c r="G231" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H231" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B232">
         <v>3.1999999999999999E-5</v>
@@ -4730,10 +4726,10 @@
         <v>16</v>
       </c>
       <c r="G232" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H232" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -4756,12 +4752,12 @@
         <v>83</v>
       </c>
       <c r="H233" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="234" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B234">
         <v>1.0400000000000001E-3</v>
@@ -4776,16 +4772,16 @@
         <v>16</v>
       </c>
       <c r="G234" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H234" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J234" s="2"/>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B235">
         <v>1.3000000000000002E-4</v>
@@ -4803,12 +4799,12 @@
         <v>35</v>
       </c>
       <c r="H235" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B236">
         <v>1.3000000000000002E-4</v>
@@ -4823,15 +4819,15 @@
         <v>16</v>
       </c>
       <c r="G236" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H236" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B237">
         <v>1.1999999999999999E-6</v>
@@ -4846,15 +4842,15 @@
         <v>16</v>
       </c>
       <c r="G237" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H237" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B238">
         <v>2.5000000000000002E-6</v>
@@ -4869,15 +4865,15 @@
         <v>16</v>
       </c>
       <c r="G238" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H238" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B239">
         <v>1.8E-3</v>
@@ -4892,10 +4888,10 @@
         <v>16</v>
       </c>
       <c r="G239" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H239" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.2">
@@ -4918,12 +4914,12 @@
         <v>38</v>
       </c>
       <c r="H240" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B241" s="6">
         <v>8.2000000000000001E-11</v>
@@ -4932,21 +4928,21 @@
         <v>18</v>
       </c>
       <c r="D241" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F241" t="s">
         <v>16</v>
       </c>
       <c r="G241" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H241" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B242">
         <v>3.3E-3</v>
@@ -4961,10 +4957,10 @@
         <v>16</v>
       </c>
       <c r="G242" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H242" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="243" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4984,10 +4980,10 @@
         <v>16</v>
       </c>
       <c r="G243" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H243" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.2">
@@ -5010,7 +5006,7 @@
         <v>32</v>
       </c>
       <c r="H244" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.2">
@@ -5033,12 +5029,12 @@
         <v>53</v>
       </c>
       <c r="H245" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B246">
         <v>1.9E-6</v>
@@ -5053,10 +5049,10 @@
         <v>16</v>
       </c>
       <c r="G246" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H246" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
@@ -5079,7 +5075,7 @@
         <v>38</v>
       </c>
       <c r="H247" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.2">
@@ -5102,7 +5098,7 @@
         <v>83</v>
       </c>
       <c r="H248" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.2">
@@ -5113,7 +5109,7 @@
         <v>-4.4000000000000003E-3</v>
       </c>
       <c r="C249" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D249" s="10" t="s">
         <v>6</v>
@@ -5122,7 +5118,7 @@
         <v>16</v>
       </c>
       <c r="G249" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H249" t="s">
         <v>81</v>
@@ -5145,7 +5141,7 @@
         <v>16</v>
       </c>
       <c r="G250" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H250" t="s">
         <v>81</v>
@@ -5154,13 +5150,13 @@
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B251">
         <v>-1.9999999999999999E-6</v>
       </c>
       <c r="C251" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D251" s="10" t="s">
         <v>6</v>
@@ -5169,7 +5165,7 @@
         <v>16</v>
       </c>
       <c r="G251" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H251" t="s">
         <v>81</v>
@@ -5177,7 +5173,7 @@
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B252">
         <v>-2.7999999999999999E-6</v>
@@ -5192,7 +5188,7 @@
         <v>16</v>
       </c>
       <c r="G252" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H252" t="s">
         <v>81</v>
@@ -5200,13 +5196,13 @@
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B253">
         <v>-1.1999999999999999E-6</v>
       </c>
       <c r="C253" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D253" s="10" t="s">
         <v>6</v>
@@ -5215,7 +5211,7 @@
         <v>16</v>
       </c>
       <c r="G253" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H253" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Fix dependency version for xarray
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-direct-air-capture.xlsx
+++ b/premise/data/additional_inventories/lci-direct-air-capture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57582260-1A4D-C64C-8C47-4E075BFF7FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFA78BA-230C-2749-9EF1-451145B58035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,10 +356,6 @@
     <t>36% PEI</t>
   </si>
   <si>
-    <t>Synthesized by impregnate amines polyethylenimine (PEI) on solid silica gel. The LCI of amine-based silica is collected from literature and based on the composition that 1 kg amine-based silica requires of 0.64kg silica
-gel and 0.36 kg PEI.</t>
-  </si>
-  <si>
     <t>carbon dioxide compression, transport and storage</t>
   </si>
   <si>
@@ -593,17 +589,22 @@
   </si>
   <si>
     <t>operational</t>
+  </si>
+  <si>
+    <t>Synthesized by impregnate amines polyethylenimine (PEI) on solid silica gel. The LCI of amine-based silica is collected from literature and based on the composition that 1 kg amine-based silica requires of 0.64kg silica
+gel and 0.36 kg PEI. Inputs of ethanol and diethyl ether are reduced by 95% to account for recovery.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -686,7 +687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -703,6 +704,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1020,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34:G42"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1219,7 +1221,7 @@
         <v>3.4369999999999998</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -1231,12 +1233,12 @@
         <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17">
         <v>4.0000000000000001E-3</v>
@@ -1251,15 +1253,15 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B18">
         <v>3.5000000000000001E-3</v>
@@ -1274,10 +1276,10 @@
         <v>16</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1300,7 +1302,7 @@
         <v>83</v>
       </c>
       <c r="H19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1311,7 +1313,7 @@
         <v>6.28</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
@@ -1320,10 +1322,10 @@
         <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1343,7 +1345,7 @@
         <v>21</v>
       </c>
       <c r="H21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1363,7 +1365,7 @@
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1371,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1463,7 +1465,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1537,7 +1539,7 @@
         <v>3.4369999999999998</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1549,12 +1551,12 @@
         <v>34</v>
       </c>
       <c r="H37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B38">
         <v>4.0000000000000001E-3</v>
@@ -1569,15 +1571,15 @@
         <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B39">
         <v>3.5000000000000001E-3</v>
@@ -1592,10 +1594,10 @@
         <v>16</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1618,7 +1620,7 @@
         <v>83</v>
       </c>
       <c r="H40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1629,7 +1631,7 @@
         <v>6.28</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D41" t="s">
         <v>24</v>
@@ -1638,15 +1640,15 @@
         <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1661,10 +1663,10 @@
         <v>16</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1684,7 +1686,7 @@
         <v>21</v>
       </c>
       <c r="H43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1704,7 +1706,7 @@
         <v>21</v>
       </c>
       <c r="H44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2215,7 +2217,7 @@
         <v>16</v>
       </c>
       <c r="G73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H73" t="s">
         <v>65</v>
@@ -2348,7 +2350,7 @@
         <v>-760000000</v>
       </c>
       <c r="C86" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
@@ -2357,7 +2359,7 @@
         <v>16</v>
       </c>
       <c r="G86" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H86" s="12"/>
       <c r="Q86" s="4"/>
@@ -2380,7 +2382,7 @@
         <v>16</v>
       </c>
       <c r="G87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H87" s="12"/>
       <c r="Q87" s="3"/>
@@ -2403,7 +2405,7 @@
         <v>16</v>
       </c>
       <c r="G88" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H88" s="12"/>
       <c r="Q88" s="3"/>
@@ -2426,7 +2428,7 @@
         <v>16</v>
       </c>
       <c r="G89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H89" s="12"/>
       <c r="I89" s="13"/>
@@ -2448,7 +2450,7 @@
         <v>16</v>
       </c>
       <c r="G90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H90" s="12"/>
     </row>
@@ -2469,7 +2471,7 @@
         <v>16</v>
       </c>
       <c r="G91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H91" s="12"/>
     </row>
@@ -2490,7 +2492,7 @@
         <v>16</v>
       </c>
       <c r="G92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H92" s="12"/>
     </row>
@@ -2523,7 +2525,7 @@
         <v>-80000000</v>
       </c>
       <c r="C94" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -2532,7 +2534,7 @@
         <v>16</v>
       </c>
       <c r="G94" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H94" s="12"/>
     </row>
@@ -2553,7 +2555,7 @@
         <v>16</v>
       </c>
       <c r="G95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H95" s="12"/>
     </row>
@@ -2562,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -2610,7 +2612,7 @@
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -2654,7 +2656,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2692,12 +2694,12 @@
         <v>86</v>
       </c>
       <c r="H108" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B109">
         <f>1/(100000000*20)</f>
@@ -2721,7 +2723,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="B110">
         <f>-1/(100000000*20)</f>
@@ -2763,7 +2765,7 @@
         <v>83</v>
       </c>
       <c r="H111" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -2774,7 +2776,7 @@
         <v>5.4</v>
       </c>
       <c r="C112" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D112" t="s">
         <v>24</v>
@@ -2783,10 +2785,10 @@
         <v>16</v>
       </c>
       <c r="G112" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H112" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -2806,7 +2808,7 @@
         <v>21</v>
       </c>
       <c r="H113" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -2826,7 +2828,7 @@
         <v>21</v>
       </c>
       <c r="H114" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2834,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -2882,7 +2884,7 @@
         <v>9</v>
       </c>
       <c r="B122" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -2926,7 +2928,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2964,12 +2966,12 @@
         <v>86</v>
       </c>
       <c r="H127" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B128">
         <f>1/(100000000*20)</f>
@@ -2993,7 +2995,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="B129">
         <f>-1/(100000000*20)</f>
@@ -3035,7 +3037,7 @@
         <v>83</v>
       </c>
       <c r="H130" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -3046,7 +3048,7 @@
         <v>5.4</v>
       </c>
       <c r="C131" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D131" t="s">
         <v>24</v>
@@ -3055,15 +3057,15 @@
         <v>16</v>
       </c>
       <c r="G131" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H131" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -3078,10 +3080,10 @@
         <v>16</v>
       </c>
       <c r="G132" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H132" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -3101,7 +3103,7 @@
         <v>21</v>
       </c>
       <c r="H133" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -3121,7 +3123,7 @@
         <v>21</v>
       </c>
       <c r="H134" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3129,7 +3131,7 @@
         <v>0</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -3177,7 +3179,7 @@
         <v>9</v>
       </c>
       <c r="B142" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -3221,7 +3223,7 @@
     </row>
     <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -3259,12 +3261,12 @@
         <v>53</v>
       </c>
       <c r="H147" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B148">
         <v>942000</v>
@@ -3282,7 +3284,7 @@
         <v>35</v>
       </c>
       <c r="H148" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -3305,12 +3307,12 @@
         <v>53</v>
       </c>
       <c r="H149" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B150">
         <v>548000.00000000012</v>
@@ -3328,7 +3330,7 @@
         <v>35</v>
       </c>
       <c r="H150" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -3351,12 +3353,12 @@
         <v>32</v>
       </c>
       <c r="H151" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B152">
         <v>16000</v>
@@ -3371,10 +3373,10 @@
         <v>16</v>
       </c>
       <c r="G152" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H152" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -3394,10 +3396,10 @@
         <v>16</v>
       </c>
       <c r="G153" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H153" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -3420,12 +3422,12 @@
         <v>54</v>
       </c>
       <c r="H154" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B155">
         <v>10000</v>
@@ -3440,15 +3442,15 @@
         <v>16</v>
       </c>
       <c r="G155" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H155" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B156">
         <v>12000</v>
@@ -3463,15 +3465,15 @@
         <v>16</v>
       </c>
       <c r="G156" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H156" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B157">
         <v>10000</v>
@@ -3486,10 +3488,10 @@
         <v>16</v>
       </c>
       <c r="G157" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H157" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -3512,12 +3514,12 @@
         <v>64</v>
       </c>
       <c r="H158" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B159">
         <v>10000</v>
@@ -3532,10 +3534,10 @@
         <v>16</v>
       </c>
       <c r="G159" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H159" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -3558,7 +3560,7 @@
         <v>54</v>
       </c>
       <c r="H160" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -3581,12 +3583,12 @@
         <v>32</v>
       </c>
       <c r="H161" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B162">
         <v>94000</v>
@@ -3601,15 +3603,15 @@
         <v>16</v>
       </c>
       <c r="G162" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H162" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B163">
         <v>10000</v>
@@ -3624,15 +3626,15 @@
         <v>16</v>
       </c>
       <c r="G163" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H163" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B164">
         <v>10000</v>
@@ -3647,10 +3649,10 @@
         <v>16</v>
       </c>
       <c r="G164" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H164" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -3673,7 +3675,7 @@
         <v>54</v>
       </c>
       <c r="H165" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
@@ -3696,7 +3698,7 @@
         <v>32</v>
       </c>
       <c r="H166" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
@@ -3707,7 +3709,7 @@
         <v>0</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -3755,7 +3757,7 @@
         <v>9</v>
       </c>
       <c r="B174" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -3799,7 +3801,7 @@
     </row>
     <row r="178" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B178">
         <v>-1</v>
@@ -3825,7 +3827,7 @@
         <v>-29400000</v>
       </c>
       <c r="C179" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D179" t="s">
         <v>6</v>
@@ -3834,7 +3836,7 @@
         <v>16</v>
       </c>
       <c r="G179" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q179" s="4"/>
       <c r="S179" s="4"/>
@@ -3856,7 +3858,7 @@
         <v>16</v>
       </c>
       <c r="G180" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q180" s="3"/>
       <c r="S180" s="3"/>
@@ -3878,7 +3880,7 @@
         <v>16</v>
       </c>
       <c r="G181" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q181" s="3"/>
       <c r="S181" s="3"/>
@@ -3911,7 +3913,7 @@
         <v>-6000000</v>
       </c>
       <c r="C183" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D183" t="s">
         <v>6</v>
@@ -3920,18 +3922,18 @@
         <v>16</v>
       </c>
       <c r="G183" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="184" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B184">
         <v>-20000</v>
       </c>
       <c r="C184" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D184" t="s">
         <v>6</v>
@@ -3940,18 +3942,18 @@
         <v>16</v>
       </c>
       <c r="G184" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="185" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B185">
         <v>-26000</v>
       </c>
       <c r="C185" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D185" t="s">
         <v>6</v>
@@ -3960,7 +3962,7 @@
         <v>16</v>
       </c>
       <c r="G185" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="186" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -4019,7 +4021,7 @@
         <v>9</v>
       </c>
       <c r="B193" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
     </row>
     <row r="194" spans="1:19" x14ac:dyDescent="0.2">
@@ -4195,7 +4197,7 @@
         <v>16</v>
       </c>
       <c r="G202" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H202" t="s">
         <v>104</v>
@@ -4204,7 +4206,7 @@
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B203">
         <v>4.1999999999999998E-5</v>
@@ -4239,7 +4241,7 @@
         <v>16</v>
       </c>
       <c r="G204" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H204" t="s">
         <v>105</v>
@@ -4285,7 +4287,7 @@
         <v>16</v>
       </c>
       <c r="G206" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H206" t="s">
         <v>105</v>
@@ -4308,7 +4310,7 @@
         <v>16</v>
       </c>
       <c r="G207" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H207" t="s">
         <v>105</v>
@@ -4319,7 +4321,8 @@
         <v>101</v>
       </c>
       <c r="B208">
-        <v>1.24</v>
+        <f>1.24*0.05</f>
+        <v>6.2E-2</v>
       </c>
       <c r="C208" t="s">
         <v>18</v>
@@ -4331,7 +4334,7 @@
         <v>16</v>
       </c>
       <c r="G208" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H208" t="s">
         <v>105</v>
@@ -4341,8 +4344,9 @@
       <c r="A209" t="s">
         <v>102</v>
       </c>
-      <c r="B209" s="2">
-        <v>14.84</v>
+      <c r="B209" s="14">
+        <f>0.36*(AVERAGE(33.94,48.48))*(1-0.97)</f>
+        <v>0.44506800000000035</v>
       </c>
       <c r="C209" t="s">
         <v>28</v>
@@ -4354,7 +4358,7 @@
         <v>16</v>
       </c>
       <c r="G209" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H209" t="s">
         <v>105</v>
@@ -4414,7 +4418,7 @@
         <v>2.69</v>
       </c>
       <c r="C212" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D212" t="s">
         <v>24</v>
@@ -4446,7 +4450,7 @@
         <v>16</v>
       </c>
       <c r="G213" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H213" t="s">
         <v>105</v>
@@ -4460,7 +4464,7 @@
         <v>-0.54</v>
       </c>
       <c r="C214" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D214" t="s">
         <v>6</v>
@@ -4469,7 +4473,7 @@
         <v>16</v>
       </c>
       <c r="G214" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H214" t="s">
         <v>105</v>
@@ -4507,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.2">
@@ -4523,7 +4527,7 @@
         <v>2</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
@@ -4555,7 +4559,7 @@
         <v>9</v>
       </c>
       <c r="B223" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.2">
@@ -4599,7 +4603,7 @@
     </row>
     <row r="227" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -4614,7 +4618,7 @@
         <v>15</v>
       </c>
       <c r="G227" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.2">
@@ -4637,12 +4641,12 @@
         <v>53</v>
       </c>
       <c r="H228" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B229">
         <v>1.0000000000000001E-7</v>
@@ -4657,10 +4661,10 @@
         <v>16</v>
       </c>
       <c r="G229" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H229" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.2">
@@ -4683,12 +4687,12 @@
         <v>32</v>
       </c>
       <c r="H230" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B231">
         <v>2.9999999999999999E-7</v>
@@ -4703,15 +4707,15 @@
         <v>16</v>
       </c>
       <c r="G231" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H231" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B232">
         <v>3.1999999999999999E-5</v>
@@ -4726,10 +4730,10 @@
         <v>16</v>
       </c>
       <c r="G232" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H232" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -4752,12 +4756,12 @@
         <v>83</v>
       </c>
       <c r="H233" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="234" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B234">
         <v>1.0400000000000001E-3</v>
@@ -4772,16 +4776,16 @@
         <v>16</v>
       </c>
       <c r="G234" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H234" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J234" s="2"/>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B235">
         <v>1.3000000000000002E-4</v>
@@ -4799,12 +4803,12 @@
         <v>35</v>
       </c>
       <c r="H235" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B236">
         <v>1.3000000000000002E-4</v>
@@ -4819,15 +4823,15 @@
         <v>16</v>
       </c>
       <c r="G236" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H236" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B237">
         <v>1.1999999999999999E-6</v>
@@ -4842,15 +4846,15 @@
         <v>16</v>
       </c>
       <c r="G237" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H237" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B238">
         <v>2.5000000000000002E-6</v>
@@ -4865,15 +4869,15 @@
         <v>16</v>
       </c>
       <c r="G238" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H238" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B239">
         <v>1.8E-3</v>
@@ -4888,10 +4892,10 @@
         <v>16</v>
       </c>
       <c r="G239" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H239" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.2">
@@ -4914,12 +4918,12 @@
         <v>38</v>
       </c>
       <c r="H240" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B241" s="6">
         <v>8.2000000000000001E-11</v>
@@ -4928,21 +4932,21 @@
         <v>18</v>
       </c>
       <c r="D241" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F241" t="s">
         <v>16</v>
       </c>
       <c r="G241" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H241" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B242">
         <v>3.3E-3</v>
@@ -4957,10 +4961,10 @@
         <v>16</v>
       </c>
       <c r="G242" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H242" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="243" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4980,10 +4984,10 @@
         <v>16</v>
       </c>
       <c r="G243" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H243" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.2">
@@ -5006,7 +5010,7 @@
         <v>32</v>
       </c>
       <c r="H244" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.2">
@@ -5029,12 +5033,12 @@
         <v>53</v>
       </c>
       <c r="H245" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B246">
         <v>1.9E-6</v>
@@ -5049,10 +5053,10 @@
         <v>16</v>
       </c>
       <c r="G246" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H246" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
@@ -5075,7 +5079,7 @@
         <v>38</v>
       </c>
       <c r="H247" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.2">
@@ -5098,7 +5102,7 @@
         <v>83</v>
       </c>
       <c r="H248" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.2">
@@ -5109,7 +5113,7 @@
         <v>-4.4000000000000003E-3</v>
       </c>
       <c r="C249" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D249" s="10" t="s">
         <v>6</v>
@@ -5118,7 +5122,7 @@
         <v>16</v>
       </c>
       <c r="G249" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H249" t="s">
         <v>81</v>
@@ -5141,7 +5145,7 @@
         <v>16</v>
       </c>
       <c r="G250" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H250" t="s">
         <v>81</v>
@@ -5150,13 +5154,13 @@
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B251">
         <v>-1.9999999999999999E-6</v>
       </c>
       <c r="C251" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D251" s="10" t="s">
         <v>6</v>
@@ -5165,7 +5169,7 @@
         <v>16</v>
       </c>
       <c r="G251" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H251" t="s">
         <v>81</v>
@@ -5173,7 +5177,7 @@
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B252">
         <v>-2.7999999999999999E-6</v>
@@ -5188,7 +5192,7 @@
         <v>16</v>
       </c>
       <c r="G252" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H252" t="s">
         <v>81</v>
@@ -5196,13 +5200,13 @@
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B253">
         <v>-1.1999999999999999E-6</v>
       </c>
       <c r="C253" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D253" s="10" t="s">
         <v>6</v>
@@ -5211,7 +5215,7 @@
         <v>16</v>
       </c>
       <c r="G253" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H253" t="s">
         <v>81</v>

</xml_diff>